<commit_message>
update Report Samples xlsx
</commit_message>
<xml_diff>
--- a/VODDAI_ReportSamples_tw.xlsx
+++ b/VODDAI_ReportSamples_tw.xlsx
@@ -2671,21 +2671,21 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="2" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="21" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5664,11 +5664,11 @@
       </c>
       <c r="C19" s="125">
         <f ca="1">C18 / RANDBETWEEN(2,4)</f>
-        <v>2500705.5</v>
+        <v>1667137</v>
       </c>
       <c r="D19" s="236">
         <f ca="1">D18 / RANDBETWEEN(2,4)</f>
-        <v>4327</v>
+        <v>3245.25</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.3">
@@ -5677,11 +5677,11 @@
       </c>
       <c r="C20" s="127">
         <f ca="1">(C18-C19) / RANDBETWEEN(2,4)</f>
-        <v>1250352.75</v>
+        <v>833568.5</v>
       </c>
       <c r="D20" s="237">
         <f ca="1">(D18-D19) / RANDBETWEEN(2,4)</f>
-        <v>2163.5</v>
+        <v>3245.25</v>
       </c>
     </row>
     <row r="21" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -5690,7 +5690,7 @@
       </c>
       <c r="C21" s="126">
         <f ca="1">C18 - (C19+C20)</f>
-        <v>1250352.75</v>
+        <v>2500705.5</v>
       </c>
       <c r="D21" s="238">
         <f ca="1">D18 - (D19+D20)</f>
@@ -5715,11 +5715,11 @@
       </c>
       <c r="C23" s="125">
         <f ca="1">C22 / RANDBETWEEN(2,4)</f>
-        <v>416784.25</v>
+        <v>625176.375</v>
       </c>
       <c r="D23" s="236">
         <f ca="1">D22 / RANDBETWEEN(2,4)</f>
-        <v>7070.666666666667</v>
+        <v>10606</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.3">
@@ -5728,11 +5728,11 @@
       </c>
       <c r="C24" s="127">
         <f ca="1">(C22-C23) / RANDBETWEEN(2,4)</f>
-        <v>277856.16666666669</v>
+        <v>312588.1875</v>
       </c>
       <c r="D24" s="237">
         <f ca="1">(D22-D23) / RANDBETWEEN(2,4)</f>
-        <v>4713.7777777777774</v>
+        <v>5303</v>
       </c>
     </row>
     <row r="25" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -5741,11 +5741,11 @@
       </c>
       <c r="C25" s="126">
         <f ca="1">C22 - (C23+C24)</f>
-        <v>555712.33333333326</v>
+        <v>312588.1875</v>
       </c>
       <c r="D25" s="238">
         <f ca="1">D22 - (D23+D24)</f>
-        <v>9427.5555555555547</v>
+        <v>5303</v>
       </c>
     </row>
     <row r="26" spans="2:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
@@ -5783,7 +5783,7 @@
       </c>
       <c r="D28" s="237">
         <f ca="1">(D26-D27) / RANDBETWEEN(2,4)</f>
-        <v>133455.75</v>
+        <v>66727.875</v>
       </c>
     </row>
     <row r="29" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -5796,7 +5796,7 @@
       </c>
       <c r="D29" s="238">
         <f ca="1">D26 - (D27+D28)</f>
-        <v>133455.75</v>
+        <v>200183.625</v>
       </c>
     </row>
     <row r="30" spans="2:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
@@ -5821,7 +5821,7 @@
       </c>
       <c r="D31" s="237">
         <f ca="1">D30 / RANDBETWEEN(2,4)</f>
-        <v>55719.25</v>
+        <v>74292.333333333328</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.3">
@@ -5830,11 +5830,11 @@
       </c>
       <c r="C32" s="127">
         <f ca="1">(C30-C31) / RANDBETWEEN(2,4)</f>
-        <v>6490.5</v>
+        <v>4867.875</v>
       </c>
       <c r="D32" s="237">
         <f ca="1">(D30-D31) / RANDBETWEEN(2,4)</f>
-        <v>83578.875</v>
+        <v>49528.222222222226</v>
       </c>
     </row>
     <row r="33" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -5843,11 +5843,11 @@
       </c>
       <c r="C33" s="126">
         <f ca="1">C30 - (C31+C32)</f>
-        <v>12981</v>
+        <v>14603.625</v>
       </c>
       <c r="D33" s="238">
         <f ca="1">D30 - (D31+D32)</f>
-        <v>83578.875</v>
+        <v>99056.444444444438</v>
       </c>
     </row>
     <row r="34" spans="2:4" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -6004,7 +6004,7 @@
       <c r="D15" s="246"/>
       <c r="E15" s="240">
         <f ca="1">E14 / RANDBETWEEN(2,4)</f>
-        <v>1250352.75</v>
+        <v>1667137</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.3">
@@ -6014,7 +6014,7 @@
       <c r="D16" s="247"/>
       <c r="E16" s="241">
         <f ca="1">(E14-E15) / RANDBETWEEN(2,4)</f>
-        <v>1250352.75</v>
+        <v>1667137</v>
       </c>
     </row>
     <row r="17" spans="3:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -6024,7 +6024,7 @@
       <c r="D17" s="248"/>
       <c r="E17" s="242">
         <f ca="1">E14 - (E15+E16)</f>
-        <v>2500705.5</v>
+        <v>1667137</v>
       </c>
     </row>
     <row r="18" spans="3:5" ht="15" thickTop="1" x14ac:dyDescent="0.3">
@@ -6124,7 +6124,7 @@
       <c r="D27" s="246"/>
       <c r="E27" s="240">
         <f ca="1">E26 / RANDBETWEEN(2,4)</f>
-        <v>177941</v>
+        <v>118627.33333333333</v>
       </c>
     </row>
     <row r="28" spans="3:5" x14ac:dyDescent="0.3">
@@ -6134,7 +6134,7 @@
       <c r="D28" s="247"/>
       <c r="E28" s="241">
         <f ca="1">(E26-E27) / RANDBETWEEN(2,4)</f>
-        <v>59313.666666666664</v>
+        <v>79084.888888888891</v>
       </c>
     </row>
     <row r="29" spans="3:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -6144,7 +6144,7 @@
       <c r="D29" s="248"/>
       <c r="E29" s="242">
         <f ca="1">E26 - (E27+E28)</f>
-        <v>118627.33333333334</v>
+        <v>158169.77777777778</v>
       </c>
     </row>
     <row r="30" spans="3:5" ht="15" thickTop="1" x14ac:dyDescent="0.3">
@@ -6164,7 +6164,7 @@
       <c r="D31" s="247"/>
       <c r="E31" s="241">
         <f ca="1">E30 / RANDBETWEEN(2,4)</f>
-        <v>74292.333333333328</v>
+        <v>55719.25</v>
       </c>
     </row>
     <row r="32" spans="3:5" x14ac:dyDescent="0.3">
@@ -6174,7 +6174,7 @@
       <c r="D32" s="247"/>
       <c r="E32" s="241">
         <f ca="1">(E30-E31) / RANDBETWEEN(2,4)</f>
-        <v>37146.166666666672</v>
+        <v>41789.4375</v>
       </c>
     </row>
     <row r="33" spans="3:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -6184,7 +6184,7 @@
       <c r="D33" s="248"/>
       <c r="E33" s="242">
         <f ca="1">E30 - (E31+E32)</f>
-        <v>111438.5</v>
+        <v>125368.3125</v>
       </c>
     </row>
     <row r="34" spans="3:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -6825,8 +6825,8 @@
   </sheetPr>
   <dimension ref="A1:AH175"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6862,7 +6862,7 @@
       <c r="K1" s="188"/>
     </row>
     <row r="2" spans="1:34" s="186" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="E2" s="311" t="s">
+      <c r="E2" s="308" t="s">
         <v>199</v>
       </c>
       <c r="G2" s="188"/>
@@ -6963,7 +6963,7 @@
     </row>
     <row r="7" spans="1:34" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="189"/>
-      <c r="B7" s="308" t="s">
+      <c r="B7" s="305" t="s">
         <v>64</v>
       </c>
       <c r="C7" s="60">
@@ -7001,7 +7001,7 @@
     </row>
     <row r="8" spans="1:34" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="189"/>
-      <c r="B8" s="308" t="s">
+      <c r="B8" s="305" t="s">
         <v>65</v>
       </c>
       <c r="C8" s="60">
@@ -7038,7 +7038,7 @@
       <c r="AH8" s="189"/>
     </row>
     <row r="9" spans="1:34" s="186" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="310" t="s">
+      <c r="B9" s="307" t="s">
         <v>196</v>
       </c>
       <c r="C9" s="186" t="s">
@@ -7062,7 +7062,7 @@
       <c r="V9" s="187"/>
     </row>
     <row r="10" spans="1:34" s="186" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="310" t="s">
+      <c r="B10" s="307" t="s">
         <v>197</v>
       </c>
       <c r="C10" s="186" t="s">
@@ -7089,7 +7089,7 @@
       <c r="V10" s="187"/>
     </row>
     <row r="11" spans="1:34" s="186" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="310" t="s">
+      <c r="B11" s="307" t="s">
         <v>198</v>
       </c>
       <c r="C11" s="186" t="s">
@@ -7123,7 +7123,7 @@
       <c r="B12" s="184" t="s">
         <v>98</v>
       </c>
-      <c r="C12" s="309" t="s">
+      <c r="C12" s="306" t="s">
         <v>126</v>
       </c>
       <c r="D12" s="185" t="s">
@@ -7294,7 +7294,7 @@
       <c r="E14" s="121"/>
       <c r="F14" s="125">
         <f ca="1">F13 / RANDBETWEEN(2,3)</f>
-        <v>2551591.3333333335</v>
+        <v>3827387</v>
       </c>
       <c r="G14" s="125">
         <f ca="1">G13 / RANDBETWEEN(2,3)</f>
@@ -7310,11 +7310,11 @@
       </c>
       <c r="J14" s="136" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>9781:9:0</v>
+        <v>14671:6:0</v>
       </c>
       <c r="K14" s="77">
         <f ca="1">K13 / RANDBETWEEN(2,3)</f>
-        <v>880299.01</v>
+        <v>586866.00666666671</v>
       </c>
       <c r="L14" s="77">
         <f ca="1">L13 / RANDBETWEEN(2,3)</f>
@@ -7322,11 +7322,11 @@
       </c>
       <c r="M14" s="77">
         <f ca="1">M13 / RANDBETWEEN(2,3)</f>
-        <v>9781</v>
+        <v>14671.5</v>
       </c>
       <c r="N14" s="77">
         <f ca="1">N13 / RANDBETWEEN(2,3)</f>
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="O14" s="77">
         <f ca="1">O13 / RANDBETWEEN(2,3)</f>
@@ -7338,7 +7338,7 @@
       </c>
       <c r="Q14" s="77">
         <f ca="1">Q13 / RANDBETWEEN(2,3)</f>
-        <v>13.8</v>
+        <v>9.2000000000000011</v>
       </c>
       <c r="R14" s="77">
         <f ca="1">R13 / RANDBETWEEN(2,3)</f>
@@ -7354,11 +7354,11 @@
       </c>
       <c r="U14" s="78" t="str">
         <f ca="1">CONCATENATE(INT(W14),":",INT(X14),":", INT(Y14))</f>
-        <v>0:1:13</v>
+        <v>0:2:9</v>
       </c>
       <c r="V14" s="298">
         <f ca="1">V13 / RANDBETWEEN(2,3)</f>
-        <v>109.1038563788584</v>
+        <v>163.6557845682876</v>
       </c>
       <c r="W14" s="299">
         <f ca="1">W13 / RANDBETWEEN(2,3)</f>
@@ -7366,11 +7366,11 @@
       </c>
       <c r="X14" s="299">
         <f ca="1">X13 / RANDBETWEEN(2,3)</f>
-        <v>1.6666666666666667</v>
+        <v>2.5</v>
       </c>
       <c r="Y14" s="299">
         <f ca="1">Y13 / RANDBETWEEN(2,3)</f>
-        <v>13.655784568287601</v>
+        <v>9.103856378858401</v>
       </c>
     </row>
     <row r="15" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -7382,7 +7382,7 @@
       <c r="E15" s="122"/>
       <c r="F15" s="126">
         <f ca="1">F13-F14</f>
-        <v>5103182.666666666</v>
+        <v>3827387</v>
       </c>
       <c r="G15" s="126">
         <f ca="1">G13-G14</f>
@@ -7398,11 +7398,11 @@
       </c>
       <c r="J15" s="137" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>19562:9:0</v>
+        <v>14671:12:0</v>
       </c>
       <c r="K15" s="87">
         <f ca="1">K13-K14</f>
-        <v>880299.01</v>
+        <v>1173732.0133333332</v>
       </c>
       <c r="L15" s="87">
         <f ca="1">L13-L14</f>
@@ -7410,11 +7410,11 @@
       </c>
       <c r="M15" s="87">
         <f ca="1">M13-M14</f>
-        <v>19562</v>
+        <v>14671.5</v>
       </c>
       <c r="N15" s="87">
         <f ca="1">N13-N14</f>
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="O15" s="87">
         <f ca="1">O13-O14</f>
@@ -7426,7 +7426,7 @@
       </c>
       <c r="Q15" s="87">
         <f ca="1">Q13-Q14</f>
-        <v>13.8</v>
+        <v>18.399999999999999</v>
       </c>
       <c r="R15" s="87">
         <f ca="1">R13-R14</f>
@@ -7442,11 +7442,11 @@
       </c>
       <c r="U15" s="88" t="str">
         <f ca="1">CONCATENATE(INT(W15),":",INT(X15),":", INT(Y15))</f>
-        <v>0:3:13</v>
+        <v>0:2:18</v>
       </c>
       <c r="V15" s="298">
         <f ca="1">V13-V14</f>
-        <v>218.20771275771682</v>
+        <v>163.6557845682876</v>
       </c>
       <c r="W15" s="299">
         <f ca="1">W13-W14</f>
@@ -7454,11 +7454,11 @@
       </c>
       <c r="X15" s="299">
         <f ca="1">X13-X14</f>
-        <v>3.333333333333333</v>
+        <v>2.5</v>
       </c>
       <c r="Y15" s="299">
         <f ca="1">Y13-Y14</f>
-        <v>13.655784568287601</v>
+        <v>18.207712757716799</v>
       </c>
     </row>
     <row r="16" spans="1:34" ht="15" thickTop="1" x14ac:dyDescent="0.3">
@@ -7562,7 +7562,7 @@
       <c r="E17" s="121"/>
       <c r="F17" s="125">
         <f ca="1">F16 / RANDBETWEEN(2,4)</f>
-        <v>413633</v>
+        <v>551510.66666666663</v>
       </c>
       <c r="G17" s="125">
         <f ca="1">G16 / RANDBETWEEN(2,4)</f>
@@ -7578,7 +7578,7 @@
       </c>
       <c r="J17" s="136" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>861:28:10</v>
+        <v>1723:28:10</v>
       </c>
       <c r="K17" s="77">
         <f ca="1">K16 / RANDBETWEEN(2,4)</f>
@@ -7586,11 +7586,11 @@
       </c>
       <c r="L17" s="77">
         <f ca="1">L16 / RANDBETWEEN(2,4)</f>
-        <v>4136330</v>
+        <v>3102247.5</v>
       </c>
       <c r="M17" s="77">
         <f ca="1">M16 / RANDBETWEEN(2,4)</f>
-        <v>861.5</v>
+        <v>1723</v>
       </c>
       <c r="N17" s="77">
         <f ca="1">N16 / RANDBETWEEN(2,4)</f>
@@ -7602,7 +7602,7 @@
       </c>
       <c r="P17" s="78" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>0:0:3</v>
+        <v>0:0:7</v>
       </c>
       <c r="Q17" s="77">
         <f ca="1">Q16 / RANDBETWEEN(2,4)</f>
@@ -7618,15 +7618,15 @@
       </c>
       <c r="T17" s="77">
         <f ca="1">T16 / RANDBETWEEN(2,4)</f>
-        <v>3.75</v>
+        <v>7.5</v>
       </c>
       <c r="U17" s="78" t="str">
         <f ca="1">CONCATENATE(INT(W17),":",INT(X17),":", INT(Y17))</f>
-        <v>0:1:28</v>
+        <v>0:0:28</v>
       </c>
       <c r="V17" s="298">
         <f ca="1">V16 / RANDBETWEEN(2,4)</f>
-        <v>59.070175939677824</v>
+        <v>44.302631954758368</v>
       </c>
       <c r="W17" s="299">
         <f ca="1">W16 / RANDBETWEEN(2,4)</f>
@@ -7634,7 +7634,7 @@
       </c>
       <c r="X17" s="299">
         <f ca="1">X16 / RANDBETWEEN(2,4)</f>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="Y17" s="299">
         <f ca="1">Y16 / RANDBETWEEN(2,4)</f>
@@ -7650,35 +7650,35 @@
       <c r="E18" s="123"/>
       <c r="F18" s="127">
         <f ca="1">(F16-F17) / RANDBETWEEN(2,4)</f>
-        <v>413633</v>
+        <v>367673.77777777781</v>
       </c>
       <c r="G18" s="127">
         <f ca="1">(G16-G17) / RANDBETWEEN(2,4)</f>
-        <v>206816.5</v>
+        <v>103408.25</v>
       </c>
       <c r="H18" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>17.721052781903349</v>
+        <v>11.814035187935565</v>
       </c>
       <c r="I18" s="127">
         <f ca="1">(I16-I17) / RANDBETWEEN(2,4)</f>
-        <v>11670.666666666666</v>
+        <v>8753</v>
       </c>
       <c r="J18" s="138" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>1292:14:5</v>
+        <v>861:14:6</v>
       </c>
       <c r="K18" s="81">
         <f ca="1">(K16-K17) / RANDBETWEEN(2,4)</f>
-        <v>51704.125</v>
+        <v>34469.416666666664</v>
       </c>
       <c r="L18" s="81">
         <f ca="1">(L16-L17) / RANDBETWEEN(2,4)</f>
-        <v>2068165</v>
+        <v>2326685.625</v>
       </c>
       <c r="M18" s="81">
         <f ca="1">(M16-M17) / RANDBETWEEN(2,4)</f>
-        <v>1292.25</v>
+        <v>861.5</v>
       </c>
       <c r="N18" s="81">
         <f ca="1">(N16-N17) / RANDBETWEEN(2,4)</f>
@@ -7686,7 +7686,7 @@
       </c>
       <c r="O18" s="81">
         <f ca="1">(O16-O17) / RANDBETWEEN(2,4)</f>
-        <v>5</v>
+        <v>6.666666666666667</v>
       </c>
       <c r="P18" s="84" t="str">
         <f t="shared" ca="1" si="2"/>
@@ -7694,7 +7694,7 @@
       </c>
       <c r="Q18" s="81">
         <f ca="1">(Q16-Q17) / RANDBETWEEN(2,4)</f>
-        <v>1.875</v>
+        <v>3.75</v>
       </c>
       <c r="R18" s="81">
         <f ca="1">(R16-R17) / RANDBETWEEN(2,4)</f>
@@ -7710,11 +7710,11 @@
       </c>
       <c r="U18" s="84" t="str">
         <f ca="1">CONCATENATE(INT(W18),":",INT(X18),":", INT(Y18))</f>
-        <v>0:0:14</v>
+        <v>0:0:9</v>
       </c>
       <c r="V18" s="298">
         <f ca="1">(V16-V17) / RANDBETWEEN(2,4)</f>
-        <v>59.070175939677824</v>
+        <v>44.302631954758368</v>
       </c>
       <c r="W18" s="299">
         <f ca="1">(W16-W17) / RANDBETWEEN(2,4)</f>
@@ -7722,11 +7722,11 @@
       </c>
       <c r="X18" s="299">
         <f ca="1">(X16-X17) / RANDBETWEEN(2,4)</f>
-        <v>0.33333333333333331</v>
+        <v>0.75</v>
       </c>
       <c r="Y18" s="299">
         <f ca="1">(Y16-Y17) / RANDBETWEEN(2,4)</f>
-        <v>14.302631954758368</v>
+        <v>9.5350879698389122</v>
       </c>
     </row>
     <row r="19" spans="2:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -7738,35 +7738,35 @@
       <c r="E19" s="122"/>
       <c r="F19" s="126">
         <f ca="1">F16 - (F17+F18)</f>
-        <v>827266</v>
+        <v>735347.5555555555</v>
       </c>
       <c r="G19" s="126">
         <f ca="1">G16 - (G17+G18)</f>
-        <v>206816.5</v>
+        <v>310224.75</v>
       </c>
       <c r="H19" s="130">
         <f t="shared" ca="1" si="0"/>
-        <v>8.8605263909516729</v>
+        <v>11.814035187935565</v>
       </c>
       <c r="I19" s="126">
         <f ca="1">I16 - (I17+I18)</f>
-        <v>23341.333333333336</v>
+        <v>26259</v>
       </c>
       <c r="J19" s="137" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>1292:14:15</v>
+        <v>861:14:13</v>
       </c>
       <c r="K19" s="87">
         <f ca="1">K16 - (K17+K18)</f>
-        <v>51704.125</v>
+        <v>68938.833333333343</v>
       </c>
       <c r="L19" s="87">
         <f ca="1">L16 - (L17+L18)</f>
-        <v>6204495</v>
+        <v>6980056.875</v>
       </c>
       <c r="M19" s="87">
         <f ca="1">M16 - (M17+M18)</f>
-        <v>1292.25</v>
+        <v>861.5</v>
       </c>
       <c r="N19" s="87">
         <f ca="1">N16 - (N17+N18)</f>
@@ -7774,15 +7774,15 @@
       </c>
       <c r="O19" s="87">
         <f ca="1">O16 - (O17+O18)</f>
-        <v>15</v>
+        <v>13.333333333333332</v>
       </c>
       <c r="P19" s="88" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>0:0:7</v>
+        <v>0:0:3</v>
       </c>
       <c r="Q19" s="87">
         <f ca="1">Q16 - (Q17+Q18)</f>
-        <v>5.625</v>
+        <v>3.75</v>
       </c>
       <c r="R19" s="87">
         <f ca="1">R16 - (R17+R18)</f>
@@ -7794,15 +7794,15 @@
       </c>
       <c r="T19" s="87">
         <f ca="1">T16 - (T17+T18)</f>
-        <v>7.5</v>
+        <v>3.75</v>
       </c>
       <c r="U19" s="88" t="str">
         <f ca="1">CONCATENATE(INT(W19),":",INT(X19),":", INT(Y19))</f>
-        <v>0:0:14</v>
+        <v>0:0:19</v>
       </c>
       <c r="V19" s="298">
         <f ca="1">V16 - (V17+V18)</f>
-        <v>59.070175939677824</v>
+        <v>88.605263909516736</v>
       </c>
       <c r="W19" s="299">
         <f ca="1">W16 - (W17+W18)</f>
@@ -7810,11 +7810,11 @@
       </c>
       <c r="X19" s="299">
         <f ca="1">X16 - (X17+X18)</f>
-        <v>0.66666666666666674</v>
+        <v>0.75</v>
       </c>
       <c r="Y19" s="299">
         <f ca="1">Y16 - (Y17+Y18)</f>
-        <v>14.302631954758368</v>
+        <v>19.070175939677824</v>
       </c>
     </row>
     <row r="20" spans="2:25" ht="15" thickTop="1" x14ac:dyDescent="0.3">
@@ -8278,43 +8278,43 @@
       <c r="E25" s="121"/>
       <c r="F25" s="125">
         <f ca="1">F24 / RANDBETWEEN(2,4)</f>
-        <v>1264972</v>
+        <v>1897458</v>
       </c>
       <c r="G25" s="125">
         <f ca="1">G24 / RANDBETWEEN(2,4)</f>
-        <v>632486</v>
+        <v>948729</v>
       </c>
       <c r="H25" s="129">
         <f t="shared" ca="1" si="0"/>
-        <v>6.2716554562131259</v>
+        <v>12.54331091242625</v>
       </c>
       <c r="I25" s="125">
         <f ca="1">I24 / RANDBETWEEN(2,4)</f>
-        <v>100848.33333333333</v>
+        <v>75636.25</v>
       </c>
       <c r="J25" s="136" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>4111:7:12</v>
+        <v>3083:9:18</v>
       </c>
       <c r="K25" s="77">
         <f ca="1">K24 / RANDBETWEEN(2,4)</f>
-        <v>246669.54</v>
+        <v>185002.155</v>
       </c>
       <c r="L25" s="77">
         <f ca="1">L24 / RANDBETWEEN(2,4)</f>
-        <v>22200258.600000001</v>
+        <v>11100129.300000001</v>
       </c>
       <c r="M25" s="77">
         <f ca="1">M24 / RANDBETWEEN(2,4)</f>
-        <v>4111</v>
+        <v>3083.25</v>
       </c>
       <c r="N25" s="77">
         <f ca="1">N24 / RANDBETWEEN(2,4)</f>
-        <v>7</v>
+        <v>9.3333333333333339</v>
       </c>
       <c r="O25" s="77">
         <f ca="1">O24 / RANDBETWEEN(2,4)</f>
-        <v>12.40000000099341</v>
+        <v>18.600000001490116</v>
       </c>
       <c r="P25" s="78" t="str">
         <f t="shared" ca="1" si="2"/>
@@ -8322,7 +8322,7 @@
       </c>
       <c r="Q25" s="77">
         <f ca="1">Q24 / RANDBETWEEN(2,4)</f>
-        <v>5.8500000000000005</v>
+        <v>11.700000000000001</v>
       </c>
       <c r="R25" s="77">
         <f ca="1">R24 / RANDBETWEEN(2,4)</f>
@@ -8338,7 +8338,7 @@
       </c>
       <c r="U25" s="78" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>0:0:8</v>
+        <v>0:0:13</v>
       </c>
       <c r="V25" s="298">
         <f ca="1">V24 / RANDBETWEEN(2,4)</f>
@@ -8350,11 +8350,11 @@
       </c>
       <c r="X25" s="299">
         <f ca="1">X24 / RANDBETWEEN(2,4)</f>
-        <v>0.5</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="Y25" s="299">
         <f ca="1">Y24 / RANDBETWEEN(2,4)</f>
-        <v>8.918912558462381</v>
+        <v>13.378368837693571</v>
       </c>
     </row>
     <row r="26" spans="2:25" x14ac:dyDescent="0.3">
@@ -8366,43 +8366,43 @@
       <c r="E26" s="123"/>
       <c r="F26" s="127">
         <f ca="1">(F24-F25) / RANDBETWEEN(2,4)</f>
-        <v>843314.66666666663</v>
+        <v>948729</v>
       </c>
       <c r="G26" s="127">
         <f ca="1">(G24-G25) / RANDBETWEEN(2,4)</f>
-        <v>421657.33333333331</v>
+        <v>237182.25</v>
       </c>
       <c r="H26" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>4.1811036374754167</v>
+        <v>3.1358277281065625</v>
       </c>
       <c r="I26" s="127">
         <f ca="1">(I24-I25) / RANDBETWEEN(2,4)</f>
-        <v>100848.33333333334</v>
+        <v>75636.25</v>
       </c>
       <c r="J26" s="138" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>2740:5:8</v>
+        <v>2312:9:9</v>
       </c>
       <c r="K26" s="81">
         <f ca="1">(K24-K25) / RANDBETWEEN(2,4)</f>
-        <v>246669.53999999998</v>
+        <v>138751.61624999999</v>
       </c>
       <c r="L26" s="81">
         <f ca="1">(L24-L25) / RANDBETWEEN(2,4)</f>
-        <v>11100129.300000001</v>
+        <v>8325096.9750000006</v>
       </c>
       <c r="M26" s="81">
         <f ca="1">(M24-M25) / RANDBETWEEN(2,4)</f>
-        <v>2740.6666666666665</v>
+        <v>2312.4375</v>
       </c>
       <c r="N26" s="81">
         <f ca="1">(N24-N25) / RANDBETWEEN(2,4)</f>
-        <v>5.25</v>
+        <v>9.3333333333333321</v>
       </c>
       <c r="O26" s="81">
         <f ca="1">(O24-O25) / RANDBETWEEN(2,4)</f>
-        <v>8.2666666673289413</v>
+        <v>9.3000000007450581</v>
       </c>
       <c r="P26" s="84" t="str">
         <f t="shared" ca="1" si="2"/>
@@ -8410,7 +8410,7 @@
       </c>
       <c r="Q26" s="81">
         <f ca="1">(Q24-Q25) / RANDBETWEEN(2,4)</f>
-        <v>8.7750000000000004</v>
+        <v>5.8500000000000005</v>
       </c>
       <c r="R26" s="81">
         <f ca="1">(R24-R25) / RANDBETWEEN(2,4)</f>
@@ -8426,11 +8426,11 @@
       </c>
       <c r="U26" s="84" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>0:0:8</v>
+        <v>0:0:3</v>
       </c>
       <c r="V26" s="298">
         <f ca="1">(V24-V25) / RANDBETWEEN(2,4)</f>
-        <v>32.612608372308252</v>
+        <v>24.45945627923119</v>
       </c>
       <c r="W26" s="299">
         <f ca="1">(W24-W25) / RANDBETWEEN(2,4)</f>
@@ -8438,11 +8438,11 @@
       </c>
       <c r="X26" s="299">
         <f ca="1">(X24-X25) / RANDBETWEEN(2,4)</f>
-        <v>0.375</v>
+        <v>0.33333333333333337</v>
       </c>
       <c r="Y26" s="299">
         <f ca="1">(Y24-Y25) / RANDBETWEEN(2,4)</f>
-        <v>8.918912558462381</v>
+        <v>3.3445922094233929</v>
       </c>
     </row>
     <row r="27" spans="2:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -8454,43 +8454,43 @@
       <c r="E27" s="122"/>
       <c r="F27" s="126">
         <f ca="1">F24 - (F25+F26)</f>
-        <v>1686629.3333333335</v>
+        <v>948729</v>
       </c>
       <c r="G27" s="126">
         <f ca="1">G24 - (G25+G26)</f>
-        <v>843314.66666666674</v>
+        <v>711546.75</v>
       </c>
       <c r="H27" s="130">
         <f t="shared" ca="1" si="0"/>
-        <v>8.3622072749508369</v>
+        <v>4.7037415921598438</v>
       </c>
       <c r="I27" s="126">
         <f ca="1">I24 - (I25+I26)</f>
-        <v>100848.33333333331</v>
+        <v>151272.5</v>
       </c>
       <c r="J27" s="137" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>5481:15:16</v>
+        <v>6937:9:9</v>
       </c>
       <c r="K27" s="87">
         <f ca="1">K24 - (K25+K26)</f>
-        <v>246669.54000000004</v>
+        <v>416254.84875</v>
       </c>
       <c r="L27" s="87">
         <f ca="1">L24 - (L25+L26)</f>
-        <v>11100129.300000001</v>
+        <v>24975290.925000001</v>
       </c>
       <c r="M27" s="87">
         <f ca="1">M24 - (M25+M26)</f>
-        <v>5481.3333333333339</v>
+        <v>6937.3125</v>
       </c>
       <c r="N27" s="87">
         <f ca="1">N24 - (N25+N26)</f>
-        <v>15.75</v>
+        <v>9.3333333333333357</v>
       </c>
       <c r="O27" s="87">
         <f ca="1">O24 - (O25+O26)</f>
-        <v>16.533333334657883</v>
+        <v>9.3000000007450581</v>
       </c>
       <c r="P27" s="88" t="str">
         <f t="shared" ca="1" si="2"/>
@@ -8498,7 +8498,7 @@
       </c>
       <c r="Q27" s="87">
         <f ca="1">Q24 - (Q25+Q26)</f>
-        <v>8.7750000000000021</v>
+        <v>5.8500000000000014</v>
       </c>
       <c r="R27" s="87">
         <f ca="1">R24 - (R25+R26)</f>
@@ -8514,11 +8514,11 @@
       </c>
       <c r="U27" s="88" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>0:1:8</v>
+        <v>0:1:10</v>
       </c>
       <c r="V27" s="298">
         <f ca="1">V24 - (V25+V26)</f>
-        <v>65.225216744616517</v>
+        <v>73.378368837693571</v>
       </c>
       <c r="W27" s="299">
         <f ca="1">W24 - (W25+W26)</f>
@@ -8526,11 +8526,11 @@
       </c>
       <c r="X27" s="299">
         <f ca="1">X24 - (X25+X26)</f>
-        <v>1.125</v>
+        <v>1</v>
       </c>
       <c r="Y27" s="299">
         <f ca="1">Y24 - (Y25+Y26)</f>
-        <v>8.918912558462381</v>
+        <v>10.033776628270179</v>
       </c>
     </row>
     <row r="28" spans="2:25" ht="15" thickTop="1" x14ac:dyDescent="0.3">
@@ -9540,7 +9540,7 @@
       <c r="V39" s="187"/>
     </row>
     <row r="40" spans="2:25" s="186" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="310"/>
+      <c r="B40" s="307"/>
       <c r="G40" s="187"/>
       <c r="H40" s="187"/>
       <c r="I40" s="187"/>
@@ -12477,7 +12477,7 @@
       <c r="D15" s="121"/>
       <c r="E15" s="125">
         <f ca="1">E14 / RANDBETWEEN(2,3)</f>
-        <v>3827387</v>
+        <v>2551591.3333333335</v>
       </c>
       <c r="F15" s="125">
         <f ca="1">F14 / RANDBETWEEN(2,3)</f>
@@ -12485,23 +12485,23 @@
       </c>
       <c r="G15" s="129">
         <f t="shared" ca="1" si="0"/>
-        <v>11.859114823788957</v>
+        <v>7.9060765491926377</v>
       </c>
       <c r="H15" s="125">
         <f ca="1">H14 / RANDBETWEEN(2,3)</f>
-        <v>107579.33333333333</v>
+        <v>161369</v>
       </c>
       <c r="I15" s="136" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>14671:6:0</v>
+        <v>14671:9:0</v>
       </c>
       <c r="J15" s="77">
         <f ca="1">J14 / RANDBETWEEN(2,3)</f>
-        <v>880299.01</v>
+        <v>586866.00666666671</v>
       </c>
       <c r="K15" s="77">
         <f ca="1">K14 / RANDBETWEEN(2,3)</f>
-        <v>35211960.399999999</v>
+        <v>52817940.600000001</v>
       </c>
       <c r="L15" s="77">
         <f ca="1">L14 / RANDBETWEEN(2,3)</f>
@@ -12509,15 +12509,15 @@
       </c>
       <c r="M15" s="77">
         <f ca="1">M14 / RANDBETWEEN(2,3)</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="N15" s="77">
         <f ca="1">N14 / RANDBETWEEN(2,3)</f>
-        <v>0.40000000099341076</v>
+        <v>0.60000000149011612</v>
       </c>
       <c r="O15" s="141" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>0:0:9</v>
+        <v>0:0:13</v>
       </c>
       <c r="P15" s="77">
         <f ca="1">P14 / RANDBETWEEN(2,3)</f>
@@ -12533,15 +12533,15 @@
       </c>
       <c r="S15" s="77">
         <f ca="1">S14 / RANDBETWEEN(2,3)</f>
-        <v>9.2000000000000011</v>
+        <v>13.8</v>
       </c>
       <c r="T15" s="78" t="str">
         <f ca="1">CONCATENATE(INT(V15),":",INT(W15),":", INT(X15))</f>
-        <v>0:1:13</v>
+        <v>0:1:9</v>
       </c>
       <c r="U15" s="77">
         <f ca="1">U14 / RANDBETWEEN(2,3)</f>
-        <v>163.6557845682876</v>
+        <v>109.1038563788584</v>
       </c>
       <c r="V15" s="77">
         <f ca="1">V14 / RANDBETWEEN(2,3)</f>
@@ -12553,7 +12553,7 @@
       </c>
       <c r="X15" s="77">
         <f ca="1">X14 / RANDBETWEEN(2,3)</f>
-        <v>13.655784568287601</v>
+        <v>9.103856378858401</v>
       </c>
       <c r="Y15" s="265"/>
     </row>
@@ -12565,7 +12565,7 @@
       <c r="D16" s="122"/>
       <c r="E16" s="126">
         <f ca="1">E14-E15</f>
-        <v>3827387</v>
+        <v>5103182.666666666</v>
       </c>
       <c r="F16" s="126">
         <f ca="1">F14-F15</f>
@@ -12573,23 +12573,23 @@
       </c>
       <c r="G16" s="130">
         <f t="shared" ca="1" si="0"/>
-        <v>11.859114823788953</v>
+        <v>15.812153098385272</v>
       </c>
       <c r="H16" s="126">
         <f ca="1">H14-H15</f>
-        <v>215158.66666666669</v>
+        <v>161369</v>
       </c>
       <c r="I16" s="137" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>14671:12:0</v>
+        <v>14671:9:0</v>
       </c>
       <c r="J16" s="87">
         <f ca="1">J14-J15</f>
-        <v>880299.01</v>
+        <v>1173732.0133333332</v>
       </c>
       <c r="K16" s="87">
         <f ca="1">K14-K15</f>
-        <v>70423920.800000012</v>
+        <v>52817940.600000001</v>
       </c>
       <c r="L16" s="87">
         <f ca="1">L14-L15</f>
@@ -12597,15 +12597,15 @@
       </c>
       <c r="M16" s="87">
         <f ca="1">M14-M15</f>
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="N16" s="87">
         <f ca="1">N14-N15</f>
-        <v>0.80000000198682142</v>
+        <v>0.60000000149011612</v>
       </c>
       <c r="O16" s="142" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>0:0:18</v>
+        <v>0:0:13</v>
       </c>
       <c r="P16" s="87">
         <f ca="1">P14-P15</f>
@@ -12621,15 +12621,15 @@
       </c>
       <c r="S16" s="87">
         <f ca="1">S14-S15</f>
-        <v>18.399999999999999</v>
+        <v>13.8</v>
       </c>
       <c r="T16" s="88" t="str">
         <f ca="1">CONCATENATE(INT(V16),":",INT(W16),":", INT(X16))</f>
-        <v>0:3:13</v>
+        <v>0:3:18</v>
       </c>
       <c r="U16" s="79">
         <f ca="1">U14-U15</f>
-        <v>163.6557845682876</v>
+        <v>218.20771275771682</v>
       </c>
       <c r="V16" s="79">
         <f ca="1">V14-V15</f>
@@ -12641,7 +12641,7 @@
       </c>
       <c r="X16" s="79">
         <f ca="1">X14-X15</f>
-        <v>13.655784568287601</v>
+        <v>18.207712757716799</v>
       </c>
       <c r="Y16" s="265"/>
     </row>
@@ -12743,27 +12743,27 @@
       <c r="D18" s="121"/>
       <c r="E18" s="125">
         <f ca="1">E17 / RANDBETWEEN(2,4)</f>
-        <v>413633</v>
+        <v>827266</v>
       </c>
       <c r="F18" s="125">
         <f ca="1">F17 / RANDBETWEEN(2,4)</f>
-        <v>206816.5</v>
+        <v>413633</v>
       </c>
       <c r="G18" s="129">
         <f t="shared" ca="1" si="0"/>
-        <v>8.8605263909516747</v>
+        <v>23.628070375871129</v>
       </c>
       <c r="H18" s="125">
         <f ca="1">H17 / RANDBETWEEN(2,4)</f>
-        <v>23341.333333333332</v>
+        <v>17506</v>
       </c>
       <c r="I18" s="136" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>861:28:10</v>
+        <v>861:14:10</v>
       </c>
       <c r="J18" s="77">
         <f ca="1">J17 / RANDBETWEEN(2,4)</f>
-        <v>68938.833333333328</v>
+        <v>51704.125</v>
       </c>
       <c r="K18" s="77">
         <f ca="1">K17 / RANDBETWEEN(2,4)</f>
@@ -12775,7 +12775,7 @@
       </c>
       <c r="M18" s="77">
         <f ca="1">M17 / RANDBETWEEN(2,4)</f>
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="N18" s="77">
         <f ca="1">N17 / RANDBETWEEN(2,4)</f>
@@ -12783,7 +12783,7 @@
       </c>
       <c r="O18" s="141" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>0:0:7</v>
+        <v>0:0:5</v>
       </c>
       <c r="P18" s="77">
         <f ca="1">P17 / RANDBETWEEN(2,4)</f>
@@ -12799,15 +12799,15 @@
       </c>
       <c r="S18" s="77">
         <f ca="1">S17 / RANDBETWEEN(2,4)</f>
-        <v>7.5</v>
+        <v>5</v>
       </c>
       <c r="T18" s="78" t="str">
         <f ca="1">CONCATENATE(INT(V18),":",INT(W18),":", INT(X18))</f>
-        <v>0:0:28</v>
+        <v>0:1:14</v>
       </c>
       <c r="U18" s="85">
         <f ca="1">U17 / RANDBETWEEN(2,4)</f>
-        <v>59.070175939677824</v>
+        <v>88.605263909516736</v>
       </c>
       <c r="V18" s="75">
         <f ca="1">V17 / RANDBETWEEN(2,4)</f>
@@ -12815,11 +12815,11 @@
       </c>
       <c r="W18" s="75">
         <f ca="1">W17 / RANDBETWEEN(2,4)</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="X18" s="263">
         <f ca="1">X17 / RANDBETWEEN(2,4)</f>
-        <v>28.605263909516736</v>
+        <v>14.302631954758368</v>
       </c>
       <c r="Y18" s="265"/>
     </row>
@@ -12831,31 +12831,31 @@
       <c r="D19" s="123"/>
       <c r="E19" s="127">
         <f ca="1">(E17-E18) / RANDBETWEEN(2,4)</f>
-        <v>413633</v>
+        <v>275755.33333333331</v>
       </c>
       <c r="F19" s="127">
         <f ca="1">(F17-F18) / RANDBETWEEN(2,4)</f>
-        <v>310224.75</v>
+        <v>206816.5</v>
       </c>
       <c r="G19" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>13.290789586427509</v>
+        <v>7.8760234586237097</v>
       </c>
       <c r="H19" s="127">
         <f ca="1">(H17-H18) / RANDBETWEEN(2,4)</f>
-        <v>23341.333333333336</v>
+        <v>26259</v>
       </c>
       <c r="I19" s="138" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>861:9:5</v>
+        <v>861:21:10</v>
       </c>
       <c r="J19" s="81">
         <f ca="1">(J17-J18) / RANDBETWEEN(2,4)</f>
-        <v>45959.222222222226</v>
+        <v>38778.09375</v>
       </c>
       <c r="K19" s="81">
         <f ca="1">(K17-K18) / RANDBETWEEN(2,4)</f>
-        <v>4653371.25</v>
+        <v>2326685.625</v>
       </c>
       <c r="L19" s="81">
         <f ca="1">(L17-L18) / RANDBETWEEN(2,4)</f>
@@ -12863,19 +12863,19 @@
       </c>
       <c r="M19" s="81">
         <f ca="1">(M17-M18) / RANDBETWEEN(2,4)</f>
-        <v>9.3333333333333339</v>
+        <v>21</v>
       </c>
       <c r="N19" s="81">
         <f ca="1">(N17-N18) / RANDBETWEEN(2,4)</f>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="O19" s="143" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>0:0:1</v>
+        <v>0:0:5</v>
       </c>
       <c r="P19" s="81">
         <f ca="1">(P17-P18) / RANDBETWEEN(2,4)</f>
-        <v>1.875</v>
+        <v>3.75</v>
       </c>
       <c r="Q19" s="81">
         <f ca="1">(Q17-Q18) / RANDBETWEEN(2,4)</f>
@@ -12887,15 +12887,15 @@
       </c>
       <c r="S19" s="81">
         <f ca="1">(S17-S18) / RANDBETWEEN(2,4)</f>
-        <v>1.875</v>
+        <v>5</v>
       </c>
       <c r="T19" s="84" t="str">
         <f ca="1">CONCATENATE(INT(V19),":",INT(W19),":", INT(X19))</f>
-        <v>0:0:14</v>
+        <v>0:0:21</v>
       </c>
       <c r="U19" s="85">
         <f ca="1">(U17-U18) / RANDBETWEEN(2,4)</f>
-        <v>39.380117293118552</v>
+        <v>44.302631954758368</v>
       </c>
       <c r="V19" s="75">
         <f ca="1">(V17-V18) / RANDBETWEEN(2,4)</f>
@@ -12907,7 +12907,7 @@
       </c>
       <c r="X19" s="263">
         <f ca="1">(X17-X18) / RANDBETWEEN(2,4)</f>
-        <v>14.302631954758368</v>
+        <v>21.453947932137552</v>
       </c>
       <c r="Y19" s="265"/>
     </row>
@@ -12919,31 +12919,31 @@
       <c r="D20" s="122"/>
       <c r="E20" s="126">
         <f ca="1">E17 - (E18+E19)</f>
-        <v>827266</v>
+        <v>551510.66666666674</v>
       </c>
       <c r="F20" s="126">
         <f ca="1">F17 - (F18+F19)</f>
-        <v>310224.75</v>
+        <v>206816.5</v>
       </c>
       <c r="G20" s="130">
         <f t="shared" ca="1" si="0"/>
-        <v>13.290789586427513</v>
+        <v>7.8760234586237097</v>
       </c>
       <c r="H20" s="126">
         <f ca="1">H17 - (H18+H19)</f>
-        <v>23341.333333333328</v>
+        <v>26259</v>
       </c>
       <c r="I20" s="137" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>1723:18:15</v>
+        <v>1723:21:10</v>
       </c>
       <c r="J20" s="87">
         <f ca="1">J17 - (J18+J19)</f>
-        <v>91918.444444444438</v>
+        <v>116334.28125</v>
       </c>
       <c r="K20" s="87">
         <f ca="1">K17 - (K18+K19)</f>
-        <v>4653371.25</v>
+        <v>6980056.875</v>
       </c>
       <c r="L20" s="87">
         <f ca="1">L17 - (L18+L19)</f>
@@ -12951,11 +12951,11 @@
       </c>
       <c r="M20" s="87">
         <f ca="1">M17 - (M18+M19)</f>
-        <v>18.666666666666664</v>
+        <v>21</v>
       </c>
       <c r="N20" s="87">
         <f ca="1">N17 - (N18+N19)</f>
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="O20" s="142" t="str">
         <f t="shared" ca="1" si="2"/>
@@ -12963,7 +12963,7 @@
       </c>
       <c r="P20" s="87">
         <f ca="1">P17 - (P18+P19)</f>
-        <v>5.625</v>
+        <v>3.75</v>
       </c>
       <c r="Q20" s="87">
         <f ca="1">Q17 - (Q18+Q19)</f>
@@ -12975,15 +12975,15 @@
       </c>
       <c r="S20" s="87">
         <f ca="1">S17 - (S18+S19)</f>
-        <v>5.625</v>
+        <v>5</v>
       </c>
       <c r="T20" s="88" t="str">
         <f ca="1">CONCATENATE(INT(V20),":",INT(W20),":", INT(X20))</f>
-        <v>0:1:14</v>
+        <v>0:0:21</v>
       </c>
       <c r="U20" s="85">
         <f ca="1">U17 - (U18+U19)</f>
-        <v>78.76023458623709</v>
+        <v>44.302631954758368</v>
       </c>
       <c r="V20" s="75">
         <f ca="1">V17 - (V18+V19)</f>
@@ -12991,11 +12991,11 @@
       </c>
       <c r="W20" s="75">
         <f ca="1">W17 - (W18+W19)</f>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="X20" s="263">
         <f ca="1">X17 - (X18+X19)</f>
-        <v>14.302631954758368</v>
+        <v>21.453947932137552</v>
       </c>
       <c r="Y20" s="265"/>
     </row>
@@ -13453,7 +13453,7 @@
       <c r="D26" s="121"/>
       <c r="E26" s="125">
         <f ca="1">E25 / RANDBETWEEN(2,4)</f>
-        <v>1897458</v>
+        <v>948729</v>
       </c>
       <c r="F26" s="125">
         <f ca="1">F25 / RANDBETWEEN(2,4)</f>
@@ -13469,11 +13469,11 @@
       </c>
       <c r="I26" s="136" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>6166:14:12</v>
+        <v>3083:9:12</v>
       </c>
       <c r="J26" s="77">
         <f ca="1">J25 / RANDBETWEEN(2,4)</f>
-        <v>185002.155</v>
+        <v>370004.31</v>
       </c>
       <c r="K26" s="77">
         <f ca="1">K25 / RANDBETWEEN(2,4)</f>
@@ -13481,11 +13481,11 @@
       </c>
       <c r="L26" s="77">
         <f ca="1">L25 / RANDBETWEEN(2,4)</f>
-        <v>6166.5</v>
+        <v>3083.25</v>
       </c>
       <c r="M26" s="77">
         <f ca="1">M25 / RANDBETWEEN(2,4)</f>
-        <v>14</v>
+        <v>9.3333333333333339</v>
       </c>
       <c r="N26" s="77">
         <f ca="1">N25 / RANDBETWEEN(2,4)</f>
@@ -13497,7 +13497,7 @@
       </c>
       <c r="P26" s="77">
         <f ca="1">P25 / RANDBETWEEN(2,4)</f>
-        <v>7.8000000000000007</v>
+        <v>11.700000000000001</v>
       </c>
       <c r="Q26" s="77">
         <f ca="1">Q25 / RANDBETWEEN(2,4)</f>
@@ -13517,7 +13517,7 @@
       </c>
       <c r="U26" s="85">
         <f ca="1">U25 / RANDBETWEEN(2,4)</f>
-        <v>48.918912558462381</v>
+        <v>36.689184418846786</v>
       </c>
       <c r="V26" s="75">
         <f ca="1">V25 / RANDBETWEEN(2,4)</f>
@@ -13541,7 +13541,7 @@
       <c r="D27" s="123"/>
       <c r="E27" s="127">
         <f ca="1">(E25-E26) / RANDBETWEEN(2,4)</f>
-        <v>948729</v>
+        <v>711546.75</v>
       </c>
       <c r="F27" s="127">
         <f ca="1">(F25-F26) / RANDBETWEEN(2,4)</f>
@@ -13549,15 +13549,15 @@
       </c>
       <c r="G27" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>5.2917092911798234</v>
+        <v>3.5278061941198828</v>
       </c>
       <c r="H27" s="127">
         <f ca="1">(H25-H26) / RANDBETWEEN(2,4)</f>
-        <v>67232.222222222234</v>
+        <v>100848.33333333334</v>
       </c>
       <c r="I27" s="138" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>1541:7:8</v>
+        <v>4624:4:12</v>
       </c>
       <c r="J27" s="81">
         <f ca="1">(J25-J26) / RANDBETWEEN(2,4)</f>
@@ -13565,27 +13565,27 @@
       </c>
       <c r="K27" s="81">
         <f ca="1">(K25-K26) / RANDBETWEEN(2,4)</f>
-        <v>11100129.300000001</v>
+        <v>16650193.950000001</v>
       </c>
       <c r="L27" s="81">
         <f ca="1">(L25-L26) / RANDBETWEEN(2,4)</f>
-        <v>1541.625</v>
+        <v>4624.875</v>
       </c>
       <c r="M27" s="81">
         <f ca="1">(M25-M26) / RANDBETWEEN(2,4)</f>
-        <v>7</v>
+        <v>4.6666666666666661</v>
       </c>
       <c r="N27" s="81">
         <f ca="1">(N25-N26) / RANDBETWEEN(2,4)</f>
-        <v>8.2666666673289413</v>
+        <v>12.400000000993412</v>
       </c>
       <c r="O27" s="143" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>0:0:5</v>
+        <v>0:0:2</v>
       </c>
       <c r="P27" s="81">
         <f ca="1">(P25-P26) / RANDBETWEEN(2,4)</f>
-        <v>3.9000000000000004</v>
+        <v>5.8500000000000005</v>
       </c>
       <c r="Q27" s="81">
         <f ca="1">(Q25-Q26) / RANDBETWEEN(2,4)</f>
@@ -13597,15 +13597,15 @@
       </c>
       <c r="S27" s="81">
         <f ca="1">(S25-S26) / RANDBETWEEN(2,4)</f>
-        <v>5.8500000000000005</v>
+        <v>2.9250000000000003</v>
       </c>
       <c r="T27" s="84" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>0:0:10</v>
+        <v>0:0:5</v>
       </c>
       <c r="U27" s="85">
         <f ca="1">(U25-U26) / RANDBETWEEN(2,4)</f>
-        <v>32.612608372308252</v>
+        <v>27.516888314135088</v>
       </c>
       <c r="V27" s="75">
         <f ca="1">(V25-V26) / RANDBETWEEN(2,4)</f>
@@ -13617,7 +13617,7 @@
       </c>
       <c r="X27" s="263">
         <f ca="1">(X25-X26) / RANDBETWEEN(2,4)</f>
-        <v>10.033776628270179</v>
+        <v>5.0168883141350893</v>
       </c>
       <c r="Y27" s="265"/>
     </row>
@@ -13629,7 +13629,7 @@
       <c r="D28" s="122"/>
       <c r="E28" s="126">
         <f ca="1">E25 - (E26+E27)</f>
-        <v>948729</v>
+        <v>2134640.25</v>
       </c>
       <c r="F28" s="126">
         <f ca="1">F25 - (F26+F27)</f>
@@ -13637,23 +13637,23 @@
       </c>
       <c r="G28" s="130">
         <f t="shared" ca="1" si="0"/>
-        <v>7.9375639367697373</v>
+        <v>10.58341858235965</v>
       </c>
       <c r="H28" s="126">
         <f ca="1">H25 - (H26+H27)</f>
-        <v>134464.44444444444</v>
+        <v>100848.33333333331</v>
       </c>
       <c r="I28" s="137" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>4624:7:16</v>
+        <v>4624:14:12</v>
       </c>
       <c r="J28" s="87">
         <f ca="1">J25 - (J26+J27)</f>
-        <v>370004.31</v>
+        <v>185002.15500000003</v>
       </c>
       <c r="K28" s="87">
         <f ca="1">K25 - (K26+K27)</f>
-        <v>22200258.600000001</v>
+        <v>16650193.950000003</v>
       </c>
       <c r="L28" s="87">
         <f ca="1">L25 - (L26+L27)</f>
@@ -13661,19 +13661,19 @@
       </c>
       <c r="M28" s="87">
         <f ca="1">M25 - (M26+M27)</f>
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="N28" s="87">
         <f ca="1">N25 - (N26+N27)</f>
-        <v>16.533333334657883</v>
+        <v>12.400000000993408</v>
       </c>
       <c r="O28" s="142" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>0:0:5</v>
+        <v>0:0:8</v>
       </c>
       <c r="P28" s="87">
         <f ca="1">P25 - (P26+P27)</f>
-        <v>11.700000000000001</v>
+        <v>5.8500000000000014</v>
       </c>
       <c r="Q28" s="87">
         <f ca="1">Q25 - (Q26+Q27)</f>
@@ -13685,15 +13685,15 @@
       </c>
       <c r="S28" s="87">
         <f ca="1">S25 - (S26+S27)</f>
-        <v>5.8500000000000014</v>
+        <v>8.7750000000000004</v>
       </c>
       <c r="T28" s="88" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>0:0:10</v>
+        <v>0:0:15</v>
       </c>
       <c r="U28" s="85">
         <f ca="1">U25 - (U26+U27)</f>
-        <v>65.225216744616517</v>
+        <v>82.550664942405263</v>
       </c>
       <c r="V28" s="75">
         <f ca="1">V25 - (V26+V27)</f>
@@ -13705,7 +13705,7 @@
       </c>
       <c r="X28" s="263">
         <f ca="1">X25 - (X26+X27)</f>
-        <v>10.033776628270179</v>
+        <v>15.050664942405268</v>
       </c>
       <c r="Y28" s="265"/>
     </row>
@@ -17412,8 +17412,8 @@
       <c r="K12" s="201"/>
       <c r="L12" s="201"/>
       <c r="M12" s="191"/>
-      <c r="N12" s="305"/>
-      <c r="O12" s="305"/>
+      <c r="N12" s="309"/>
+      <c r="O12" s="309"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="186"/>
@@ -17738,10 +17738,10 @@
       <c r="C20" s="186"/>
       <c r="D20" s="186"/>
       <c r="E20" s="186"/>
-      <c r="F20" s="306" t="s">
+      <c r="F20" s="310" t="s">
         <v>124</v>
       </c>
-      <c r="G20" s="307"/>
+      <c r="G20" s="311"/>
       <c r="H20" s="202" t="s">
         <v>79</v>
       </c>
@@ -18090,8 +18090,8 @@
       <c r="L11" s="201"/>
       <c r="M11" s="201"/>
       <c r="N11" s="191"/>
-      <c r="O11" s="305"/>
-      <c r="P11" s="305"/>
+      <c r="O11" s="309"/>
+      <c r="P11" s="309"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="186"/>
@@ -18437,10 +18437,10 @@
       <c r="D19" s="186"/>
       <c r="E19" s="186"/>
       <c r="F19" s="186"/>
-      <c r="G19" s="306" t="s">
+      <c r="G19" s="310" t="s">
         <v>124</v>
       </c>
-      <c r="H19" s="307"/>
+      <c r="H19" s="311"/>
       <c r="I19" s="202" t="s">
         <v>79</v>
       </c>

</xml_diff>

<commit_message>
update VODDAI remote repo 04-Jun-2012
</commit_message>
<xml_diff>
--- a/VODDAI_ReportSamples_tw.xlsx
+++ b/VODDAI_ReportSamples_tw.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="408" windowWidth="14640" windowHeight="7536" tabRatio="874" activeTab="4"/>
+    <workbookView xWindow="480" yWindow="468" windowWidth="14640" windowHeight="7476" tabRatio="874" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Report Summary" sheetId="23" r:id="rId1"/>
@@ -5613,7 +5613,7 @@
       </c>
       <c r="C15" s="125">
         <f ca="1">C14 / RANDBETWEEN(2,4)</f>
-        <v>3334274</v>
+        <v>5001411</v>
       </c>
       <c r="D15" s="236">
         <f ca="1">D14 / RANDBETWEEN(2,4)</f>
@@ -5626,11 +5626,11 @@
       </c>
       <c r="C16" s="127">
         <f ca="1">(C14-C15) / RANDBETWEEN(2,4)</f>
-        <v>1667137</v>
+        <v>2500705.5</v>
       </c>
       <c r="D16" s="237">
         <f ca="1">(D14-D15) / RANDBETWEEN(2,4)</f>
-        <v>625176.375</v>
+        <v>833568.5</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -5639,11 +5639,11 @@
       </c>
       <c r="C17" s="126">
         <f ca="1">C14 - (C15+C16)</f>
-        <v>5001411</v>
+        <v>2500705.5</v>
       </c>
       <c r="D17" s="238">
         <f ca="1">D14 - (D15+D16)</f>
-        <v>1875529.125</v>
+        <v>1667137</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
@@ -5664,11 +5664,11 @@
       </c>
       <c r="C19" s="125">
         <f ca="1">C18 / RANDBETWEEN(2,4)</f>
-        <v>1667137</v>
+        <v>2500705.5</v>
       </c>
       <c r="D19" s="236">
         <f ca="1">D18 / RANDBETWEEN(2,4)</f>
-        <v>3245.25</v>
+        <v>6490.5</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.3">
@@ -5690,11 +5690,11 @@
       </c>
       <c r="C21" s="126">
         <f ca="1">C18 - (C19+C20)</f>
-        <v>2500705.5</v>
+        <v>1667137</v>
       </c>
       <c r="D21" s="238">
         <f ca="1">D18 - (D19+D20)</f>
-        <v>6490.5</v>
+        <v>3245.25</v>
       </c>
     </row>
     <row r="22" spans="2:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
@@ -5703,7 +5703,7 @@
       </c>
       <c r="C22" s="228">
         <f ca="1">D16*RANDBETWEEN(1.3,2.5)</f>
-        <v>1250352.75</v>
+        <v>1667137</v>
       </c>
       <c r="D22" s="223">
         <v>21212</v>
@@ -5715,11 +5715,11 @@
       </c>
       <c r="C23" s="125">
         <f ca="1">C22 / RANDBETWEEN(2,4)</f>
-        <v>625176.375</v>
+        <v>416784.25</v>
       </c>
       <c r="D23" s="236">
         <f ca="1">D22 / RANDBETWEEN(2,4)</f>
-        <v>10606</v>
+        <v>5303</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.3">
@@ -5732,7 +5732,7 @@
       </c>
       <c r="D24" s="237">
         <f ca="1">(D22-D23) / RANDBETWEEN(2,4)</f>
-        <v>5303</v>
+        <v>7954.5</v>
       </c>
     </row>
     <row r="25" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -5741,11 +5741,11 @@
       </c>
       <c r="C25" s="126">
         <f ca="1">C22 - (C23+C24)</f>
-        <v>312588.1875</v>
+        <v>937764.5625</v>
       </c>
       <c r="D25" s="238">
         <f ca="1">D22 - (D23+D24)</f>
-        <v>5303</v>
+        <v>7954.5</v>
       </c>
     </row>
     <row r="26" spans="2:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
@@ -5754,7 +5754,7 @@
       </c>
       <c r="C26" s="228">
         <f ca="1">D17*RANDBETWEEN(1.3,2.5)</f>
-        <v>3751058.25</v>
+        <v>3334274</v>
       </c>
       <c r="D26" s="223">
         <v>355882</v>
@@ -5766,11 +5766,11 @@
       </c>
       <c r="C27" s="125">
         <f ca="1">C26 / RANDBETWEEN(2,4)</f>
-        <v>1875529.125</v>
+        <v>833568.5</v>
       </c>
       <c r="D27" s="236">
         <f ca="1">D26 / RANDBETWEEN(2,4)</f>
-        <v>88970.5</v>
+        <v>118627.33333333333</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.3">
@@ -5783,7 +5783,7 @@
       </c>
       <c r="D28" s="237">
         <f ca="1">(D26-D27) / RANDBETWEEN(2,4)</f>
-        <v>66727.875</v>
+        <v>79084.888888888891</v>
       </c>
     </row>
     <row r="29" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -5792,11 +5792,11 @@
       </c>
       <c r="C29" s="126">
         <f ca="1">C26 - (C27+C28)</f>
-        <v>1250352.75</v>
+        <v>1875529.125</v>
       </c>
       <c r="D29" s="238">
         <f ca="1">D26 - (D27+D28)</f>
-        <v>200183.625</v>
+        <v>158169.77777777778</v>
       </c>
     </row>
     <row r="30" spans="2:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
@@ -5817,7 +5817,7 @@
       </c>
       <c r="C31" s="127">
         <f ca="1">C30 / RANDBETWEEN(2,4)</f>
-        <v>6490.5</v>
+        <v>8654</v>
       </c>
       <c r="D31" s="237">
         <f ca="1">D30 / RANDBETWEEN(2,4)</f>
@@ -5830,11 +5830,11 @@
       </c>
       <c r="C32" s="127">
         <f ca="1">(C30-C31) / RANDBETWEEN(2,4)</f>
-        <v>4867.875</v>
+        <v>5769.333333333333</v>
       </c>
       <c r="D32" s="237">
         <f ca="1">(D30-D31) / RANDBETWEEN(2,4)</f>
-        <v>49528.222222222226</v>
+        <v>37146.166666666672</v>
       </c>
     </row>
     <row r="33" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -5843,11 +5843,11 @@
       </c>
       <c r="C33" s="126">
         <f ca="1">C30 - (C31+C32)</f>
-        <v>14603.625</v>
+        <v>11538.666666666668</v>
       </c>
       <c r="D33" s="238">
         <f ca="1">D30 - (D31+D32)</f>
-        <v>99056.444444444438</v>
+        <v>111438.5</v>
       </c>
     </row>
     <row r="34" spans="2:4" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -6004,7 +6004,7 @@
       <c r="D15" s="246"/>
       <c r="E15" s="240">
         <f ca="1">E14 / RANDBETWEEN(2,4)</f>
-        <v>1667137</v>
+        <v>2500705.5</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.3">
@@ -6014,7 +6014,7 @@
       <c r="D16" s="247"/>
       <c r="E16" s="241">
         <f ca="1">(E14-E15) / RANDBETWEEN(2,4)</f>
-        <v>1667137</v>
+        <v>1250352.75</v>
       </c>
     </row>
     <row r="17" spans="3:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -6024,7 +6024,7 @@
       <c r="D17" s="248"/>
       <c r="E17" s="242">
         <f ca="1">E14 - (E15+E16)</f>
-        <v>1667137</v>
+        <v>1250352.75</v>
       </c>
     </row>
     <row r="18" spans="3:5" ht="15" thickTop="1" x14ac:dyDescent="0.3">
@@ -6044,7 +6044,7 @@
       <c r="D19" s="246"/>
       <c r="E19" s="240">
         <f ca="1">E18 / RANDBETWEEN(2,4)</f>
-        <v>3245.25</v>
+        <v>4327</v>
       </c>
     </row>
     <row r="20" spans="3:5" x14ac:dyDescent="0.3">
@@ -6054,7 +6054,7 @@
       <c r="D20" s="247"/>
       <c r="E20" s="241">
         <f ca="1">(E18-E19) / RANDBETWEEN(2,4)</f>
-        <v>2433.9375</v>
+        <v>4327</v>
       </c>
     </row>
     <row r="21" spans="3:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -6064,7 +6064,7 @@
       <c r="D21" s="248"/>
       <c r="E21" s="242">
         <f ca="1">E18 - (E19+E20)</f>
-        <v>7301.8125</v>
+        <v>4327</v>
       </c>
     </row>
     <row r="22" spans="3:5" ht="15" thickTop="1" x14ac:dyDescent="0.3">
@@ -6084,7 +6084,7 @@
       <c r="D23" s="246"/>
       <c r="E23" s="240">
         <f ca="1">E22 / RANDBETWEEN(2,4)</f>
-        <v>7070.666666666667</v>
+        <v>10606</v>
       </c>
     </row>
     <row r="24" spans="3:5" x14ac:dyDescent="0.3">
@@ -6094,7 +6094,7 @@
       <c r="D24" s="247"/>
       <c r="E24" s="241">
         <f ca="1">(E22-E23) / RANDBETWEEN(2,4)</f>
-        <v>3535.333333333333</v>
+        <v>2651.5</v>
       </c>
     </row>
     <row r="25" spans="3:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -6104,7 +6104,7 @@
       <c r="D25" s="248"/>
       <c r="E25" s="242">
         <f ca="1">E22 - (E23+E24)</f>
-        <v>10606</v>
+        <v>7954.5</v>
       </c>
     </row>
     <row r="26" spans="3:5" ht="15" thickTop="1" x14ac:dyDescent="0.3">
@@ -6164,7 +6164,7 @@
       <c r="D31" s="247"/>
       <c r="E31" s="241">
         <f ca="1">E30 / RANDBETWEEN(2,4)</f>
-        <v>55719.25</v>
+        <v>74292.333333333328</v>
       </c>
     </row>
     <row r="32" spans="3:5" x14ac:dyDescent="0.3">
@@ -6174,7 +6174,7 @@
       <c r="D32" s="247"/>
       <c r="E32" s="241">
         <f ca="1">(E30-E31) / RANDBETWEEN(2,4)</f>
-        <v>41789.4375</v>
+        <v>37146.166666666672</v>
       </c>
     </row>
     <row r="33" spans="3:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -6184,7 +6184,7 @@
       <c r="D33" s="248"/>
       <c r="E33" s="242">
         <f ca="1">E30 - (E31+E32)</f>
-        <v>125368.3125</v>
+        <v>111438.5</v>
       </c>
     </row>
     <row r="34" spans="3:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -6826,7 +6826,7 @@
   <dimension ref="A1:AH175"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7294,7 +7294,7 @@
       <c r="E14" s="121"/>
       <c r="F14" s="125">
         <f ca="1">F13 / RANDBETWEEN(2,3)</f>
-        <v>3827387</v>
+        <v>2551591.3333333335</v>
       </c>
       <c r="G14" s="125">
         <f ca="1">G13 / RANDBETWEEN(2,3)</f>
@@ -7310,11 +7310,11 @@
       </c>
       <c r="J14" s="136" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>14671:6:0</v>
+        <v>9781:9:0</v>
       </c>
       <c r="K14" s="77">
         <f ca="1">K13 / RANDBETWEEN(2,3)</f>
-        <v>586866.00666666671</v>
+        <v>880299.01</v>
       </c>
       <c r="L14" s="77">
         <f ca="1">L13 / RANDBETWEEN(2,3)</f>
@@ -7322,11 +7322,11 @@
       </c>
       <c r="M14" s="77">
         <f ca="1">M13 / RANDBETWEEN(2,3)</f>
-        <v>14671.5</v>
+        <v>9781</v>
       </c>
       <c r="N14" s="77">
         <f ca="1">N13 / RANDBETWEEN(2,3)</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="O14" s="77">
         <f ca="1">O13 / RANDBETWEEN(2,3)</f>
@@ -7334,11 +7334,11 @@
       </c>
       <c r="P14" s="78" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>0:0:13</v>
+        <v>0:0:9</v>
       </c>
       <c r="Q14" s="77">
         <f ca="1">Q13 / RANDBETWEEN(2,3)</f>
-        <v>9.2000000000000011</v>
+        <v>13.8</v>
       </c>
       <c r="R14" s="77">
         <f ca="1">R13 / RANDBETWEEN(2,3)</f>
@@ -7350,15 +7350,15 @@
       </c>
       <c r="T14" s="77">
         <f ca="1">T13 / RANDBETWEEN(2,3)</f>
-        <v>13.8</v>
+        <v>9.2000000000000011</v>
       </c>
       <c r="U14" s="78" t="str">
         <f ca="1">CONCATENATE(INT(W14),":",INT(X14),":", INT(Y14))</f>
-        <v>0:2:9</v>
+        <v>0:1:9</v>
       </c>
       <c r="V14" s="298">
         <f ca="1">V13 / RANDBETWEEN(2,3)</f>
-        <v>163.6557845682876</v>
+        <v>109.1038563788584</v>
       </c>
       <c r="W14" s="299">
         <f ca="1">W13 / RANDBETWEEN(2,3)</f>
@@ -7366,7 +7366,7 @@
       </c>
       <c r="X14" s="299">
         <f ca="1">X13 / RANDBETWEEN(2,3)</f>
-        <v>2.5</v>
+        <v>1.6666666666666667</v>
       </c>
       <c r="Y14" s="299">
         <f ca="1">Y13 / RANDBETWEEN(2,3)</f>
@@ -7382,7 +7382,7 @@
       <c r="E15" s="122"/>
       <c r="F15" s="126">
         <f ca="1">F13-F14</f>
-        <v>3827387</v>
+        <v>5103182.666666666</v>
       </c>
       <c r="G15" s="126">
         <f ca="1">G13-G14</f>
@@ -7398,11 +7398,11 @@
       </c>
       <c r="J15" s="137" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>14671:12:0</v>
+        <v>19562:9:0</v>
       </c>
       <c r="K15" s="87">
         <f ca="1">K13-K14</f>
-        <v>1173732.0133333332</v>
+        <v>880299.01</v>
       </c>
       <c r="L15" s="87">
         <f ca="1">L13-L14</f>
@@ -7410,11 +7410,11 @@
       </c>
       <c r="M15" s="87">
         <f ca="1">M13-M14</f>
-        <v>14671.5</v>
+        <v>19562</v>
       </c>
       <c r="N15" s="87">
         <f ca="1">N13-N14</f>
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="O15" s="87">
         <f ca="1">O13-O14</f>
@@ -7422,11 +7422,11 @@
       </c>
       <c r="P15" s="88" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>0:0:13</v>
+        <v>0:0:18</v>
       </c>
       <c r="Q15" s="87">
         <f ca="1">Q13-Q14</f>
-        <v>18.399999999999999</v>
+        <v>13.8</v>
       </c>
       <c r="R15" s="87">
         <f ca="1">R13-R14</f>
@@ -7438,15 +7438,15 @@
       </c>
       <c r="T15" s="87">
         <f ca="1">T13-T14</f>
-        <v>13.8</v>
+        <v>18.399999999999999</v>
       </c>
       <c r="U15" s="88" t="str">
         <f ca="1">CONCATENATE(INT(W15),":",INT(X15),":", INT(Y15))</f>
-        <v>0:2:18</v>
+        <v>0:3:18</v>
       </c>
       <c r="V15" s="298">
         <f ca="1">V13-V14</f>
-        <v>163.6557845682876</v>
+        <v>218.20771275771682</v>
       </c>
       <c r="W15" s="299">
         <f ca="1">W13-W14</f>
@@ -7454,7 +7454,7 @@
       </c>
       <c r="X15" s="299">
         <f ca="1">X13-X14</f>
-        <v>2.5</v>
+        <v>3.333333333333333</v>
       </c>
       <c r="Y15" s="299">
         <f ca="1">Y13-Y14</f>
@@ -7562,7 +7562,7 @@
       <c r="E17" s="121"/>
       <c r="F17" s="125">
         <f ca="1">F16 / RANDBETWEEN(2,4)</f>
-        <v>551510.66666666663</v>
+        <v>827266</v>
       </c>
       <c r="G17" s="125">
         <f ca="1">G16 / RANDBETWEEN(2,4)</f>
@@ -7570,31 +7570,31 @@
       </c>
       <c r="H17" s="129">
         <f t="shared" ca="1" si="0"/>
-        <v>11.814035187935565</v>
+        <v>17.721052781903349</v>
       </c>
       <c r="I17" s="125">
         <f ca="1">I16 / RANDBETWEEN(2,4)</f>
-        <v>35012</v>
+        <v>23341.333333333332</v>
       </c>
       <c r="J17" s="136" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>1723:28:10</v>
+        <v>861:14:10</v>
       </c>
       <c r="K17" s="77">
         <f ca="1">K16 / RANDBETWEEN(2,4)</f>
-        <v>103408.25</v>
+        <v>68938.833333333328</v>
       </c>
       <c r="L17" s="77">
         <f ca="1">L16 / RANDBETWEEN(2,4)</f>
-        <v>3102247.5</v>
+        <v>6204495</v>
       </c>
       <c r="M17" s="77">
         <f ca="1">M16 / RANDBETWEEN(2,4)</f>
-        <v>1723</v>
+        <v>861.5</v>
       </c>
       <c r="N17" s="77">
         <f ca="1">N16 / RANDBETWEEN(2,4)</f>
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="O17" s="77">
         <f ca="1">O16 / RANDBETWEEN(2,4)</f>
@@ -7622,11 +7622,11 @@
       </c>
       <c r="U17" s="78" t="str">
         <f ca="1">CONCATENATE(INT(W17),":",INT(X17),":", INT(Y17))</f>
-        <v>0:0:28</v>
+        <v>0:1:28</v>
       </c>
       <c r="V17" s="298">
         <f ca="1">V16 / RANDBETWEEN(2,4)</f>
-        <v>44.302631954758368</v>
+        <v>59.070175939677824</v>
       </c>
       <c r="W17" s="299">
         <f ca="1">W16 / RANDBETWEEN(2,4)</f>
@@ -7634,7 +7634,7 @@
       </c>
       <c r="X17" s="299">
         <f ca="1">X16 / RANDBETWEEN(2,4)</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="Y17" s="299">
         <f ca="1">Y16 / RANDBETWEEN(2,4)</f>
@@ -7650,31 +7650,31 @@
       <c r="E18" s="123"/>
       <c r="F18" s="127">
         <f ca="1">(F16-F17) / RANDBETWEEN(2,4)</f>
-        <v>367673.77777777781</v>
+        <v>206816.5</v>
       </c>
       <c r="G18" s="127">
         <f ca="1">(G16-G17) / RANDBETWEEN(2,4)</f>
-        <v>103408.25</v>
+        <v>137877.66666666666</v>
       </c>
       <c r="H18" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>11.814035187935565</v>
+        <v>11.814035187935563</v>
       </c>
       <c r="I18" s="127">
         <f ca="1">(I16-I17) / RANDBETWEEN(2,4)</f>
-        <v>8753</v>
+        <v>11670.666666666668</v>
       </c>
       <c r="J18" s="138" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>861:14:6</v>
+        <v>861:21:6</v>
       </c>
       <c r="K18" s="81">
         <f ca="1">(K16-K17) / RANDBETWEEN(2,4)</f>
-        <v>34469.416666666664</v>
+        <v>45959.222222222226</v>
       </c>
       <c r="L18" s="81">
         <f ca="1">(L16-L17) / RANDBETWEEN(2,4)</f>
-        <v>2326685.625</v>
+        <v>1551123.75</v>
       </c>
       <c r="M18" s="81">
         <f ca="1">(M16-M17) / RANDBETWEEN(2,4)</f>
@@ -7682,7 +7682,7 @@
       </c>
       <c r="N18" s="81">
         <f ca="1">(N16-N17) / RANDBETWEEN(2,4)</f>
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="O18" s="81">
         <f ca="1">(O16-O17) / RANDBETWEEN(2,4)</f>
@@ -7690,7 +7690,7 @@
       </c>
       <c r="P18" s="84" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>0:0:3</v>
+        <v>0:0:2</v>
       </c>
       <c r="Q18" s="81">
         <f ca="1">(Q16-Q17) / RANDBETWEEN(2,4)</f>
@@ -7706,7 +7706,7 @@
       </c>
       <c r="T18" s="81">
         <f ca="1">(T16-T17) / RANDBETWEEN(2,4)</f>
-        <v>3.75</v>
+        <v>2.5</v>
       </c>
       <c r="U18" s="84" t="str">
         <f ca="1">CONCATENATE(INT(W18),":",INT(X18),":", INT(Y18))</f>
@@ -7714,7 +7714,7 @@
       </c>
       <c r="V18" s="298">
         <f ca="1">(V16-V17) / RANDBETWEEN(2,4)</f>
-        <v>44.302631954758368</v>
+        <v>59.070175939677824</v>
       </c>
       <c r="W18" s="299">
         <f ca="1">(W16-W17) / RANDBETWEEN(2,4)</f>
@@ -7722,7 +7722,7 @@
       </c>
       <c r="X18" s="299">
         <f ca="1">(X16-X17) / RANDBETWEEN(2,4)</f>
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="Y18" s="299">
         <f ca="1">(Y16-Y17) / RANDBETWEEN(2,4)</f>
@@ -7738,39 +7738,39 @@
       <c r="E19" s="122"/>
       <c r="F19" s="126">
         <f ca="1">F16 - (F17+F18)</f>
-        <v>735347.5555555555</v>
+        <v>620449.5</v>
       </c>
       <c r="G19" s="126">
         <f ca="1">G16 - (G17+G18)</f>
-        <v>310224.75</v>
+        <v>275755.33333333337</v>
       </c>
       <c r="H19" s="130">
         <f t="shared" ca="1" si="0"/>
-        <v>11.814035187935565</v>
+        <v>7.8760234586237114</v>
       </c>
       <c r="I19" s="126">
         <f ca="1">I16 - (I17+I18)</f>
-        <v>26259</v>
+        <v>35012</v>
       </c>
       <c r="J19" s="137" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>861:14:13</v>
+        <v>1723:21:13</v>
       </c>
       <c r="K19" s="87">
         <f ca="1">K16 - (K17+K18)</f>
-        <v>68938.833333333343</v>
+        <v>91918.444444444438</v>
       </c>
       <c r="L19" s="87">
         <f ca="1">L16 - (L17+L18)</f>
-        <v>6980056.875</v>
+        <v>4653371.25</v>
       </c>
       <c r="M19" s="87">
         <f ca="1">M16 - (M17+M18)</f>
-        <v>861.5</v>
+        <v>1723</v>
       </c>
       <c r="N19" s="87">
         <f ca="1">N16 - (N17+N18)</f>
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="O19" s="87">
         <f ca="1">O16 - (O17+O18)</f>
@@ -7778,7 +7778,7 @@
       </c>
       <c r="P19" s="88" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>0:0:3</v>
+        <v>0:0:5</v>
       </c>
       <c r="Q19" s="87">
         <f ca="1">Q16 - (Q17+Q18)</f>
@@ -7794,7 +7794,7 @@
       </c>
       <c r="T19" s="87">
         <f ca="1">T16 - (T17+T18)</f>
-        <v>3.75</v>
+        <v>5</v>
       </c>
       <c r="U19" s="88" t="str">
         <f ca="1">CONCATENATE(INT(W19),":",INT(X19),":", INT(Y19))</f>
@@ -7802,7 +7802,7 @@
       </c>
       <c r="V19" s="298">
         <f ca="1">V16 - (V17+V18)</f>
-        <v>88.605263909516736</v>
+        <v>59.070175939677824</v>
       </c>
       <c r="W19" s="299">
         <f ca="1">W16 - (W17+W18)</f>
@@ -8282,11 +8282,11 @@
       </c>
       <c r="G25" s="125">
         <f ca="1">G24 / RANDBETWEEN(2,4)</f>
-        <v>948729</v>
+        <v>632486</v>
       </c>
       <c r="H25" s="129">
         <f t="shared" ca="1" si="0"/>
-        <v>12.54331091242625</v>
+        <v>8.3622072749508334</v>
       </c>
       <c r="I25" s="125">
         <f ca="1">I24 / RANDBETWEEN(2,4)</f>
@@ -8294,15 +8294,15 @@
       </c>
       <c r="J25" s="136" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>3083:9:18</v>
+        <v>3083:14:9</v>
       </c>
       <c r="K25" s="77">
         <f ca="1">K24 / RANDBETWEEN(2,4)</f>
-        <v>185002.155</v>
+        <v>246669.54</v>
       </c>
       <c r="L25" s="77">
         <f ca="1">L24 / RANDBETWEEN(2,4)</f>
-        <v>11100129.300000001</v>
+        <v>14800172.4</v>
       </c>
       <c r="M25" s="77">
         <f ca="1">M24 / RANDBETWEEN(2,4)</f>
@@ -8310,15 +8310,15 @@
       </c>
       <c r="N25" s="77">
         <f ca="1">N24 / RANDBETWEEN(2,4)</f>
-        <v>9.3333333333333339</v>
+        <v>14</v>
       </c>
       <c r="O25" s="77">
         <f ca="1">O24 / RANDBETWEEN(2,4)</f>
-        <v>18.600000001490116</v>
+        <v>9.3000000007450581</v>
       </c>
       <c r="P25" s="78" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>0:0:7</v>
+        <v>0:0:5</v>
       </c>
       <c r="Q25" s="77">
         <f ca="1">Q24 / RANDBETWEEN(2,4)</f>
@@ -8334,15 +8334,15 @@
       </c>
       <c r="T25" s="77">
         <f ca="1">T24 / RANDBETWEEN(2,4)</f>
-        <v>7.8000000000000007</v>
+        <v>5.8500000000000005</v>
       </c>
       <c r="U25" s="78" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>0:0:13</v>
+        <v>0:0:8</v>
       </c>
       <c r="V25" s="298">
         <f ca="1">V24 / RANDBETWEEN(2,4)</f>
-        <v>48.918912558462381</v>
+        <v>36.689184418846786</v>
       </c>
       <c r="W25" s="299">
         <f ca="1">W24 / RANDBETWEEN(2,4)</f>
@@ -8354,7 +8354,7 @@
       </c>
       <c r="Y25" s="299">
         <f ca="1">Y24 / RANDBETWEEN(2,4)</f>
-        <v>13.378368837693571</v>
+        <v>8.918912558462381</v>
       </c>
     </row>
     <row r="26" spans="2:25" x14ac:dyDescent="0.3">
@@ -8366,39 +8366,39 @@
       <c r="E26" s="123"/>
       <c r="F26" s="127">
         <f ca="1">(F24-F25) / RANDBETWEEN(2,4)</f>
-        <v>948729</v>
+        <v>474364.5</v>
       </c>
       <c r="G26" s="127">
         <f ca="1">(G24-G25) / RANDBETWEEN(2,4)</f>
-        <v>237182.25</v>
+        <v>632486</v>
       </c>
       <c r="H26" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>3.1358277281065625</v>
+        <v>5.5748048499672223</v>
       </c>
       <c r="I26" s="127">
         <f ca="1">(I24-I25) / RANDBETWEEN(2,4)</f>
-        <v>75636.25</v>
+        <v>113454.375</v>
       </c>
       <c r="J26" s="138" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>2312:9:9</v>
+        <v>3083:3:9</v>
       </c>
       <c r="K26" s="81">
         <f ca="1">(K24-K25) / RANDBETWEEN(2,4)</f>
-        <v>138751.61624999999</v>
+        <v>246669.53999999998</v>
       </c>
       <c r="L26" s="81">
         <f ca="1">(L24-L25) / RANDBETWEEN(2,4)</f>
-        <v>8325096.9750000006</v>
+        <v>14800172.400000002</v>
       </c>
       <c r="M26" s="81">
         <f ca="1">(M24-M25) / RANDBETWEEN(2,4)</f>
-        <v>2312.4375</v>
+        <v>3083.25</v>
       </c>
       <c r="N26" s="81">
         <f ca="1">(N24-N25) / RANDBETWEEN(2,4)</f>
-        <v>9.3333333333333321</v>
+        <v>3.5</v>
       </c>
       <c r="O26" s="81">
         <f ca="1">(O24-O25) / RANDBETWEEN(2,4)</f>
@@ -8406,11 +8406,11 @@
       </c>
       <c r="P26" s="84" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>0:0:3</v>
+        <v>0:0:8</v>
       </c>
       <c r="Q26" s="81">
         <f ca="1">(Q24-Q25) / RANDBETWEEN(2,4)</f>
-        <v>5.8500000000000005</v>
+        <v>3.9000000000000004</v>
       </c>
       <c r="R26" s="81">
         <f ca="1">(R24-R25) / RANDBETWEEN(2,4)</f>
@@ -8422,15 +8422,15 @@
       </c>
       <c r="T26" s="81">
         <f ca="1">(T24-T25) / RANDBETWEEN(2,4)</f>
-        <v>3.9000000000000004</v>
+        <v>8.7750000000000004</v>
       </c>
       <c r="U26" s="84" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>0:0:3</v>
+        <v>0:0:5</v>
       </c>
       <c r="V26" s="298">
         <f ca="1">(V24-V25) / RANDBETWEEN(2,4)</f>
-        <v>24.45945627923119</v>
+        <v>55.033776628270175</v>
       </c>
       <c r="W26" s="299">
         <f ca="1">(W24-W25) / RANDBETWEEN(2,4)</f>
@@ -8442,7 +8442,7 @@
       </c>
       <c r="Y26" s="299">
         <f ca="1">(Y24-Y25) / RANDBETWEEN(2,4)</f>
-        <v>3.3445922094233929</v>
+        <v>5.9459417056415873</v>
       </c>
     </row>
     <row r="27" spans="2:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -8454,51 +8454,51 @@
       <c r="E27" s="122"/>
       <c r="F27" s="126">
         <f ca="1">F24 - (F25+F26)</f>
-        <v>948729</v>
+        <v>1423093.5</v>
       </c>
       <c r="G27" s="126">
         <f ca="1">G24 - (G25+G26)</f>
-        <v>711546.75</v>
+        <v>632486</v>
       </c>
       <c r="H27" s="130">
         <f t="shared" ca="1" si="0"/>
-        <v>4.7037415921598438</v>
+        <v>5.5748048499672223</v>
       </c>
       <c r="I27" s="126">
         <f ca="1">I24 - (I25+I26)</f>
-        <v>151272.5</v>
+        <v>113454.375</v>
       </c>
       <c r="J27" s="137" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>6937:9:9</v>
+        <v>6166:10:18</v>
       </c>
       <c r="K27" s="87">
         <f ca="1">K24 - (K25+K26)</f>
-        <v>416254.84875</v>
+        <v>246669.54000000004</v>
       </c>
       <c r="L27" s="87">
         <f ca="1">L24 - (L25+L26)</f>
-        <v>24975290.925000001</v>
+        <v>14800172.399999999</v>
       </c>
       <c r="M27" s="87">
         <f ca="1">M24 - (M25+M26)</f>
-        <v>6937.3125</v>
+        <v>6166.5</v>
       </c>
       <c r="N27" s="87">
         <f ca="1">N24 - (N25+N26)</f>
-        <v>9.3333333333333357</v>
+        <v>10.5</v>
       </c>
       <c r="O27" s="87">
         <f ca="1">O24 - (O25+O26)</f>
-        <v>9.3000000007450581</v>
+        <v>18.600000001490116</v>
       </c>
       <c r="P27" s="88" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>0:0:11</v>
+        <v>0:0:8</v>
       </c>
       <c r="Q27" s="87">
         <f ca="1">Q24 - (Q25+Q26)</f>
-        <v>5.8500000000000014</v>
+        <v>7.8000000000000007</v>
       </c>
       <c r="R27" s="87">
         <f ca="1">R24 - (R25+R26)</f>
@@ -8510,15 +8510,15 @@
       </c>
       <c r="T27" s="87">
         <f ca="1">T24 - (T25+T26)</f>
-        <v>11.700000000000001</v>
+        <v>8.7750000000000021</v>
       </c>
       <c r="U27" s="88" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>0:1:10</v>
+        <v>0:1:11</v>
       </c>
       <c r="V27" s="298">
         <f ca="1">V24 - (V25+V26)</f>
-        <v>73.378368837693571</v>
+        <v>55.033776628270175</v>
       </c>
       <c r="W27" s="299">
         <f ca="1">W24 - (W25+W26)</f>
@@ -8530,7 +8530,7 @@
       </c>
       <c r="Y27" s="299">
         <f ca="1">Y24 - (Y25+Y26)</f>
-        <v>10.033776628270179</v>
+        <v>11.891883411283175</v>
       </c>
     </row>
     <row r="28" spans="2:25" ht="15" thickTop="1" x14ac:dyDescent="0.3">
@@ -9457,7 +9457,7 @@
       </c>
       <c r="J38" s="104" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>156881:18:27</v>
+        <v>156881:18:26</v>
       </c>
       <c r="K38" s="107">
         <f ca="1">SUM(K13:K36)</f>
@@ -9465,7 +9465,7 @@
       </c>
       <c r="L38" s="107">
         <f ca="1">SUM(L13:L36)</f>
-        <v>564772707</v>
+        <v>564772706.99999988</v>
       </c>
       <c r="M38" s="105">
         <f ca="1">INT(L38/3600)</f>
@@ -9477,7 +9477,7 @@
       </c>
       <c r="O38" s="105">
         <f ca="1" xml:space="preserve"> MOD(MOD(L38, 3600),60)</f>
-        <v>27</v>
+        <v>26.99999988079071</v>
       </c>
       <c r="P38" s="109" t="str">
         <f t="shared" ca="1" si="2"/>
@@ -9485,7 +9485,7 @@
       </c>
       <c r="Q38" s="266">
         <f ca="1">L38/G38</f>
-        <v>48.716099421873778</v>
+        <v>48.716099421873764</v>
       </c>
       <c r="R38" s="105">
         <f ca="1">INT(Q38/3600)</f>
@@ -9497,7 +9497,7 @@
       </c>
       <c r="T38" s="105">
         <f ca="1" xml:space="preserve"> MOD(MOD(Q38, 3600),60)</f>
-        <v>48.716099421873778</v>
+        <v>48.716099421873764</v>
       </c>
       <c r="U38" s="109" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -9505,7 +9505,7 @@
       </c>
       <c r="V38" s="296">
         <f ca="1">L38/I38</f>
-        <v>236.6857643479868</v>
+        <v>236.68576434798675</v>
       </c>
       <c r="W38" s="297">
         <f ca="1">INT(V38/3600)</f>
@@ -9517,7 +9517,7 @@
       </c>
       <c r="Y38" s="297">
         <f ca="1" xml:space="preserve"> MOD(MOD(V38, 3600),60)</f>
-        <v>56.685764347986805</v>
+        <v>56.685764347986748</v>
       </c>
     </row>
     <row r="39" spans="2:25" s="186" customFormat="1" x14ac:dyDescent="0.3">
@@ -12006,7 +12006,9 @@
   </sheetPr>
   <dimension ref="A1:AG176"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -12477,7 +12479,7 @@
       <c r="D15" s="121"/>
       <c r="E15" s="125">
         <f ca="1">E14 / RANDBETWEEN(2,3)</f>
-        <v>2551591.3333333335</v>
+        <v>3827387</v>
       </c>
       <c r="F15" s="125">
         <f ca="1">F14 / RANDBETWEEN(2,3)</f>
@@ -12493,7 +12495,7 @@
       </c>
       <c r="I15" s="136" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>14671:9:0</v>
+        <v>9781:6:0</v>
       </c>
       <c r="J15" s="77">
         <f ca="1">J14 / RANDBETWEEN(2,3)</f>
@@ -12501,23 +12503,23 @@
       </c>
       <c r="K15" s="77">
         <f ca="1">K14 / RANDBETWEEN(2,3)</f>
-        <v>52817940.600000001</v>
+        <v>35211960.399999999</v>
       </c>
       <c r="L15" s="77">
         <f ca="1">L14 / RANDBETWEEN(2,3)</f>
-        <v>14671.5</v>
+        <v>9781</v>
       </c>
       <c r="M15" s="77">
         <f ca="1">M14 / RANDBETWEEN(2,3)</f>
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="N15" s="77">
         <f ca="1">N14 / RANDBETWEEN(2,3)</f>
-        <v>0.60000000149011612</v>
+        <v>0.40000000099341076</v>
       </c>
       <c r="O15" s="141" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>0:0:13</v>
+        <v>0:0:9</v>
       </c>
       <c r="P15" s="77">
         <f ca="1">P14 / RANDBETWEEN(2,3)</f>
@@ -12533,7 +12535,7 @@
       </c>
       <c r="S15" s="77">
         <f ca="1">S14 / RANDBETWEEN(2,3)</f>
-        <v>13.8</v>
+        <v>9.2000000000000011</v>
       </c>
       <c r="T15" s="78" t="str">
         <f ca="1">CONCATENATE(INT(V15),":",INT(W15),":", INT(X15))</f>
@@ -12565,7 +12567,7 @@
       <c r="D16" s="122"/>
       <c r="E16" s="126">
         <f ca="1">E14-E15</f>
-        <v>5103182.666666666</v>
+        <v>3827387</v>
       </c>
       <c r="F16" s="126">
         <f ca="1">F14-F15</f>
@@ -12581,7 +12583,7 @@
       </c>
       <c r="I16" s="137" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>14671:9:0</v>
+        <v>19562:12:0</v>
       </c>
       <c r="J16" s="87">
         <f ca="1">J14-J15</f>
@@ -12589,23 +12591,23 @@
       </c>
       <c r="K16" s="87">
         <f ca="1">K14-K15</f>
-        <v>52817940.600000001</v>
+        <v>70423920.800000012</v>
       </c>
       <c r="L16" s="87">
         <f ca="1">L14-L15</f>
-        <v>14671.5</v>
+        <v>19562</v>
       </c>
       <c r="M16" s="87">
         <f ca="1">M14-M15</f>
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="N16" s="87">
         <f ca="1">N14-N15</f>
-        <v>0.60000000149011612</v>
+        <v>0.80000000198682142</v>
       </c>
       <c r="O16" s="142" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>0:0:13</v>
+        <v>0:0:18</v>
       </c>
       <c r="P16" s="87">
         <f ca="1">P14-P15</f>
@@ -12621,7 +12623,7 @@
       </c>
       <c r="S16" s="87">
         <f ca="1">S14-S15</f>
-        <v>13.8</v>
+        <v>18.399999999999999</v>
       </c>
       <c r="T16" s="88" t="str">
         <f ca="1">CONCATENATE(INT(V16),":",INT(W16),":", INT(X16))</f>
@@ -12747,31 +12749,31 @@
       </c>
       <c r="F18" s="125">
         <f ca="1">F17 / RANDBETWEEN(2,4)</f>
-        <v>413633</v>
+        <v>206816.5</v>
       </c>
       <c r="G18" s="129">
         <f t="shared" ca="1" si="0"/>
-        <v>23.628070375871129</v>
+        <v>8.8605263909516747</v>
       </c>
       <c r="H18" s="125">
         <f ca="1">H17 / RANDBETWEEN(2,4)</f>
-        <v>17506</v>
+        <v>23341.333333333332</v>
       </c>
       <c r="I18" s="136" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>861:14:10</v>
+        <v>1148:14:15</v>
       </c>
       <c r="J18" s="77">
         <f ca="1">J17 / RANDBETWEEN(2,4)</f>
-        <v>51704.125</v>
+        <v>103408.25</v>
       </c>
       <c r="K18" s="77">
         <f ca="1">K17 / RANDBETWEEN(2,4)</f>
-        <v>3102247.5</v>
+        <v>6204495</v>
       </c>
       <c r="L18" s="77">
         <f ca="1">L17 / RANDBETWEEN(2,4)</f>
-        <v>861.5</v>
+        <v>1148.6666666666667</v>
       </c>
       <c r="M18" s="77">
         <f ca="1">M17 / RANDBETWEEN(2,4)</f>
@@ -12779,7 +12781,7 @@
       </c>
       <c r="N18" s="77">
         <f ca="1">N17 / RANDBETWEEN(2,4)</f>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="O18" s="141" t="str">
         <f t="shared" ca="1" si="2"/>
@@ -12803,7 +12805,7 @@
       </c>
       <c r="T18" s="78" t="str">
         <f ca="1">CONCATENATE(INT(V18),":",INT(W18),":", INT(X18))</f>
-        <v>0:1:14</v>
+        <v>0:0:28</v>
       </c>
       <c r="U18" s="85">
         <f ca="1">U17 / RANDBETWEEN(2,4)</f>
@@ -12815,11 +12817,11 @@
       </c>
       <c r="W18" s="75">
         <f ca="1">W17 / RANDBETWEEN(2,4)</f>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="X18" s="263">
         <f ca="1">X17 / RANDBETWEEN(2,4)</f>
-        <v>14.302631954758368</v>
+        <v>28.605263909516736</v>
       </c>
       <c r="Y18" s="265"/>
     </row>
@@ -12831,7 +12833,7 @@
       <c r="D19" s="123"/>
       <c r="E19" s="127">
         <f ca="1">(E17-E18) / RANDBETWEEN(2,4)</f>
-        <v>275755.33333333331</v>
+        <v>413633</v>
       </c>
       <c r="F19" s="127">
         <f ca="1">(F17-F18) / RANDBETWEEN(2,4)</f>
@@ -12839,27 +12841,27 @@
       </c>
       <c r="G19" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>7.8760234586237097</v>
+        <v>8.8605263909516729</v>
       </c>
       <c r="H19" s="127">
         <f ca="1">(H17-H18) / RANDBETWEEN(2,4)</f>
-        <v>26259</v>
+        <v>23341.333333333336</v>
       </c>
       <c r="I19" s="138" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>861:21:10</v>
+        <v>765:21:5</v>
       </c>
       <c r="J19" s="81">
         <f ca="1">(J17-J18) / RANDBETWEEN(2,4)</f>
-        <v>38778.09375</v>
+        <v>25852.0625</v>
       </c>
       <c r="K19" s="81">
         <f ca="1">(K17-K18) / RANDBETWEEN(2,4)</f>
-        <v>2326685.625</v>
+        <v>2068165</v>
       </c>
       <c r="L19" s="81">
         <f ca="1">(L17-L18) / RANDBETWEEN(2,4)</f>
-        <v>861.5</v>
+        <v>765.77777777777771</v>
       </c>
       <c r="M19" s="81">
         <f ca="1">(M17-M18) / RANDBETWEEN(2,4)</f>
@@ -12867,11 +12869,11 @@
       </c>
       <c r="N19" s="81">
         <f ca="1">(N17-N18) / RANDBETWEEN(2,4)</f>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="O19" s="143" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>0:0:5</v>
+        <v>0:0:2</v>
       </c>
       <c r="P19" s="81">
         <f ca="1">(P17-P18) / RANDBETWEEN(2,4)</f>
@@ -12887,11 +12889,11 @@
       </c>
       <c r="S19" s="81">
         <f ca="1">(S17-S18) / RANDBETWEEN(2,4)</f>
-        <v>5</v>
+        <v>2.5</v>
       </c>
       <c r="T19" s="84" t="str">
         <f ca="1">CONCATENATE(INT(V19),":",INT(W19),":", INT(X19))</f>
-        <v>0:0:21</v>
+        <v>0:0:14</v>
       </c>
       <c r="U19" s="85">
         <f ca="1">(U17-U18) / RANDBETWEEN(2,4)</f>
@@ -12903,11 +12905,11 @@
       </c>
       <c r="W19" s="75">
         <f ca="1">(W17-W18) / RANDBETWEEN(2,4)</f>
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="X19" s="263">
         <f ca="1">(X17-X18) / RANDBETWEEN(2,4)</f>
-        <v>21.453947932137552</v>
+        <v>14.302631954758368</v>
       </c>
       <c r="Y19" s="265"/>
     </row>
@@ -12919,35 +12921,35 @@
       <c r="D20" s="122"/>
       <c r="E20" s="126">
         <f ca="1">E17 - (E18+E19)</f>
-        <v>551510.66666666674</v>
+        <v>413633</v>
       </c>
       <c r="F20" s="126">
         <f ca="1">F17 - (F18+F19)</f>
-        <v>206816.5</v>
+        <v>413633</v>
       </c>
       <c r="G20" s="130">
         <f t="shared" ca="1" si="0"/>
-        <v>7.8760234586237097</v>
+        <v>17.721052781903349</v>
       </c>
       <c r="H20" s="126">
         <f ca="1">H17 - (H18+H19)</f>
-        <v>26259</v>
+        <v>23341.333333333328</v>
       </c>
       <c r="I20" s="137" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>1723:21:10</v>
+        <v>1531:21:10</v>
       </c>
       <c r="J20" s="87">
         <f ca="1">J17 - (J18+J19)</f>
-        <v>116334.28125</v>
+        <v>77556.1875</v>
       </c>
       <c r="K20" s="87">
         <f ca="1">K17 - (K18+K19)</f>
-        <v>6980056.875</v>
+        <v>4136330</v>
       </c>
       <c r="L20" s="87">
         <f ca="1">L17 - (L18+L19)</f>
-        <v>1723</v>
+        <v>1531.5555555555557</v>
       </c>
       <c r="M20" s="87">
         <f ca="1">M17 - (M18+M19)</f>
@@ -12959,7 +12961,7 @@
       </c>
       <c r="O20" s="142" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>0:0:5</v>
+        <v>0:0:7</v>
       </c>
       <c r="P20" s="87">
         <f ca="1">P17 - (P18+P19)</f>
@@ -12975,11 +12977,11 @@
       </c>
       <c r="S20" s="87">
         <f ca="1">S17 - (S18+S19)</f>
-        <v>5</v>
+        <v>7.5</v>
       </c>
       <c r="T20" s="88" t="str">
         <f ca="1">CONCATENATE(INT(V20),":",INT(W20),":", INT(X20))</f>
-        <v>0:0:21</v>
+        <v>0:0:14</v>
       </c>
       <c r="U20" s="85">
         <f ca="1">U17 - (U18+U19)</f>
@@ -12991,11 +12993,11 @@
       </c>
       <c r="W20" s="75">
         <f ca="1">W17 - (W18+W19)</f>
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="X20" s="263">
         <f ca="1">X17 - (X18+X19)</f>
-        <v>21.453947932137552</v>
+        <v>14.302631954758368</v>
       </c>
       <c r="Y20" s="265"/>
     </row>
@@ -13453,19 +13455,19 @@
       <c r="D26" s="121"/>
       <c r="E26" s="125">
         <f ca="1">E25 / RANDBETWEEN(2,4)</f>
-        <v>948729</v>
+        <v>1897458</v>
       </c>
       <c r="F26" s="125">
         <f ca="1">F25 / RANDBETWEEN(2,4)</f>
-        <v>474364.5</v>
+        <v>948729</v>
       </c>
       <c r="G26" s="129">
         <f t="shared" ca="1" si="0"/>
-        <v>4.7037415921598438</v>
+        <v>6.271655456213125</v>
       </c>
       <c r="H26" s="125">
         <f ca="1">H25 / RANDBETWEEN(2,4)</f>
-        <v>100848.33333333333</v>
+        <v>151272.5</v>
       </c>
       <c r="I26" s="136" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -13473,11 +13475,11 @@
       </c>
       <c r="J26" s="77">
         <f ca="1">J25 / RANDBETWEEN(2,4)</f>
-        <v>370004.31</v>
+        <v>246669.54</v>
       </c>
       <c r="K26" s="77">
         <f ca="1">K25 / RANDBETWEEN(2,4)</f>
-        <v>11100129.300000001</v>
+        <v>14800172.4</v>
       </c>
       <c r="L26" s="77">
         <f ca="1">L25 / RANDBETWEEN(2,4)</f>
@@ -13493,11 +13495,11 @@
       </c>
       <c r="O26" s="141" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>0:0:11</v>
+        <v>0:0:7</v>
       </c>
       <c r="P26" s="77">
         <f ca="1">P25 / RANDBETWEEN(2,4)</f>
-        <v>11.700000000000001</v>
+        <v>7.8000000000000007</v>
       </c>
       <c r="Q26" s="77">
         <f ca="1">Q25 / RANDBETWEEN(2,4)</f>
@@ -13509,11 +13511,11 @@
       </c>
       <c r="S26" s="77">
         <f ca="1">S25 / RANDBETWEEN(2,4)</f>
-        <v>11.700000000000001</v>
+        <v>7.8000000000000007</v>
       </c>
       <c r="T26" s="78" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>0:1:6</v>
+        <v>0:0:13</v>
       </c>
       <c r="U26" s="85">
         <f ca="1">U25 / RANDBETWEEN(2,4)</f>
@@ -13525,11 +13527,11 @@
       </c>
       <c r="W26" s="75">
         <f ca="1">W25 / RANDBETWEEN(2,4)</f>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="X26" s="263">
         <f ca="1">X25 / RANDBETWEEN(2,4)</f>
-        <v>6.6891844188467857</v>
+        <v>13.378368837693571</v>
       </c>
       <c r="Y26" s="265"/>
     </row>
@@ -13541,39 +13543,39 @@
       <c r="D27" s="123"/>
       <c r="E27" s="127">
         <f ca="1">(E25-E26) / RANDBETWEEN(2,4)</f>
-        <v>711546.75</v>
+        <v>632486</v>
       </c>
       <c r="F27" s="127">
         <f ca="1">(F25-F26) / RANDBETWEEN(2,4)</f>
-        <v>355773.375</v>
+        <v>474364.5</v>
       </c>
       <c r="G27" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>3.5278061941198828</v>
+        <v>9.4074831843196876</v>
       </c>
       <c r="H27" s="127">
         <f ca="1">(H25-H26) / RANDBETWEEN(2,4)</f>
-        <v>100848.33333333334</v>
+        <v>50424.166666666664</v>
       </c>
       <c r="I27" s="138" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>4624:4:12</v>
+        <v>3083:9:12</v>
       </c>
       <c r="J27" s="81">
         <f ca="1">(J25-J26) / RANDBETWEEN(2,4)</f>
-        <v>185002.155</v>
+        <v>164446.35999999999</v>
       </c>
       <c r="K27" s="81">
         <f ca="1">(K25-K26) / RANDBETWEEN(2,4)</f>
-        <v>16650193.950000001</v>
+        <v>7400086.2000000011</v>
       </c>
       <c r="L27" s="81">
         <f ca="1">(L25-L26) / RANDBETWEEN(2,4)</f>
-        <v>4624.875</v>
+        <v>3083.25</v>
       </c>
       <c r="M27" s="81">
         <f ca="1">(M25-M26) / RANDBETWEEN(2,4)</f>
-        <v>4.6666666666666661</v>
+        <v>9.3333333333333321</v>
       </c>
       <c r="N27" s="81">
         <f ca="1">(N25-N26) / RANDBETWEEN(2,4)</f>
@@ -13581,11 +13583,11 @@
       </c>
       <c r="O27" s="143" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>0:0:2</v>
+        <v>0:0:5</v>
       </c>
       <c r="P27" s="81">
         <f ca="1">(P25-P26) / RANDBETWEEN(2,4)</f>
-        <v>5.8500000000000005</v>
+        <v>3.9000000000000004</v>
       </c>
       <c r="Q27" s="81">
         <f ca="1">(Q25-Q26) / RANDBETWEEN(2,4)</f>
@@ -13597,15 +13599,15 @@
       </c>
       <c r="S27" s="81">
         <f ca="1">(S25-S26) / RANDBETWEEN(2,4)</f>
-        <v>2.9250000000000003</v>
+        <v>5.2</v>
       </c>
       <c r="T27" s="84" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>0:0:5</v>
+        <v>0:0:3</v>
       </c>
       <c r="U27" s="85">
         <f ca="1">(U25-U26) / RANDBETWEEN(2,4)</f>
-        <v>27.516888314135088</v>
+        <v>36.689184418846786</v>
       </c>
       <c r="V27" s="75">
         <f ca="1">(V25-V26) / RANDBETWEEN(2,4)</f>
@@ -13613,11 +13615,11 @@
       </c>
       <c r="W27" s="75">
         <f ca="1">(W25-W26) / RANDBETWEEN(2,4)</f>
-        <v>0.25</v>
+        <v>0.75</v>
       </c>
       <c r="X27" s="263">
         <f ca="1">(X25-X26) / RANDBETWEEN(2,4)</f>
-        <v>5.0168883141350893</v>
+        <v>3.3445922094233929</v>
       </c>
       <c r="Y27" s="265"/>
     </row>
@@ -13629,39 +13631,39 @@
       <c r="D28" s="122"/>
       <c r="E28" s="126">
         <f ca="1">E25 - (E26+E27)</f>
-        <v>2134640.25</v>
+        <v>1264972</v>
       </c>
       <c r="F28" s="126">
         <f ca="1">F25 - (F26+F27)</f>
-        <v>1067320.125</v>
+        <v>474364.5</v>
       </c>
       <c r="G28" s="130">
         <f t="shared" ca="1" si="0"/>
-        <v>10.58341858235965</v>
+        <v>4.7037415921598438</v>
       </c>
       <c r="H28" s="126">
         <f ca="1">H25 - (H26+H27)</f>
-        <v>100848.33333333331</v>
+        <v>100848.33333333334</v>
       </c>
       <c r="I28" s="137" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>4624:14:12</v>
+        <v>6166:9:12</v>
       </c>
       <c r="J28" s="87">
         <f ca="1">J25 - (J26+J27)</f>
-        <v>185002.15500000003</v>
+        <v>328892.71999999997</v>
       </c>
       <c r="K28" s="87">
         <f ca="1">K25 - (K26+K27)</f>
-        <v>16650193.950000003</v>
+        <v>22200258.600000001</v>
       </c>
       <c r="L28" s="87">
         <f ca="1">L25 - (L26+L27)</f>
-        <v>4624.875</v>
+        <v>6166.5</v>
       </c>
       <c r="M28" s="87">
         <f ca="1">M25 - (M26+M27)</f>
-        <v>14</v>
+        <v>9.3333333333333357</v>
       </c>
       <c r="N28" s="87">
         <f ca="1">N25 - (N26+N27)</f>
@@ -13669,11 +13671,11 @@
       </c>
       <c r="O28" s="142" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>0:0:8</v>
+        <v>0:0:10</v>
       </c>
       <c r="P28" s="87">
         <f ca="1">P25 - (P26+P27)</f>
-        <v>5.8500000000000014</v>
+        <v>11.700000000000001</v>
       </c>
       <c r="Q28" s="87">
         <f ca="1">Q25 - (Q26+Q27)</f>
@@ -13685,15 +13687,15 @@
       </c>
       <c r="S28" s="87">
         <f ca="1">S25 - (S26+S27)</f>
-        <v>8.7750000000000004</v>
+        <v>10.400000000000002</v>
       </c>
       <c r="T28" s="88" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>0:0:15</v>
+        <v>0:0:10</v>
       </c>
       <c r="U28" s="85">
         <f ca="1">U25 - (U26+U27)</f>
-        <v>82.550664942405263</v>
+        <v>73.378368837693571</v>
       </c>
       <c r="V28" s="75">
         <f ca="1">V25 - (V26+V27)</f>
@@ -13705,7 +13707,7 @@
       </c>
       <c r="X28" s="263">
         <f ca="1">X25 - (X26+X27)</f>
-        <v>15.050664942405268</v>
+        <v>10.033776628270179</v>
       </c>
       <c r="Y28" s="265"/>
     </row>

</xml_diff>